<commit_message>
[DOC] 수삽 비용 table 추가
</commit_message>
<xml_diff>
--- a/Femto Project 비용 List.xlsx
+++ b/Femto Project 비용 List.xlsx
@@ -8,20 +8,21 @@
   </bookViews>
   <sheets>
     <sheet name="개발비" sheetId="7" r:id="rId1"/>
-    <sheet name="부품 구입비" sheetId="9" r:id="rId2"/>
-    <sheet name="Transformer" sheetId="1" r:id="rId3"/>
-    <sheet name="0314" sheetId="8" r:id="rId4"/>
-    <sheet name="0403" sheetId="10" r:id="rId5"/>
+    <sheet name="작업비" sheetId="11" r:id="rId2"/>
+    <sheet name="부품 구입비" sheetId="9" r:id="rId3"/>
+    <sheet name="Transformer" sheetId="1" r:id="rId4"/>
+    <sheet name="0314" sheetId="8" r:id="rId5"/>
+    <sheet name="0403" sheetId="10" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3">'0314'!$B$4:$F$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4">'0314'!$B$4:$F$4</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="318">
   <si>
     <t>Vendor</t>
   </si>
@@ -1131,18 +1132,95 @@
     <t>실험실에서 사용할 장비 및 Pipette 관련 추가 부품</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
+  <si>
+    <t>부자재</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>수삽</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>개인</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Point</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>단가</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>금액</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>소계</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>작업내용</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>수량</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>합계</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>이윤</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>제이엘텍</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>SMD</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Metal mask</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sample용 견적</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>부품비</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>LF Generator MCU Board</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;?_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
     <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="0.0"/>
+    <numFmt numFmtId="181" formatCode="0\ &quot;%&quot;"/>
   </numFmts>
   <fonts count="32" x14ac:knownFonts="1">
     <font>
@@ -2300,7 +2378,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="280">
+  <cellXfs count="300">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
@@ -2901,36 +2979,76 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="78" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="41" fontId="26" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="26" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="26" fillId="33" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="41" fontId="26" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="80">
     <cellStyle name="20% - 강조색1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3316,8 +3434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B6:O34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:XFD44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3342,28 +3460,28 @@
     </row>
     <row r="8" spans="2:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="272" t="s">
+      <c r="B9" s="275" t="s">
         <v>97</v>
       </c>
       <c r="C9" s="273"/>
-      <c r="D9" s="276" t="s">
+      <c r="D9" s="270" t="s">
         <v>87</v>
       </c>
-      <c r="E9" s="276"/>
-      <c r="F9" s="276"/>
+      <c r="E9" s="270"/>
+      <c r="F9" s="270"/>
       <c r="G9" s="273" t="s">
         <v>91</v>
       </c>
       <c r="H9" s="273" t="s">
         <v>92</v>
       </c>
-      <c r="I9" s="277" t="s">
+      <c r="I9" s="271" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="10" spans="2:14" s="141" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="274"/>
-      <c r="C10" s="275"/>
+      <c r="B10" s="277"/>
+      <c r="C10" s="274"/>
       <c r="D10" s="142" t="s">
         <v>88</v>
       </c>
@@ -3373,24 +3491,24 @@
       <c r="F10" s="142" t="s">
         <v>90</v>
       </c>
-      <c r="G10" s="275"/>
-      <c r="H10" s="275"/>
-      <c r="I10" s="278"/>
+      <c r="G10" s="274"/>
+      <c r="H10" s="274"/>
+      <c r="I10" s="272"/>
     </row>
     <row r="11" spans="2:14" s="141" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="270" t="s">
+      <c r="B11" s="278" t="s">
         <v>102</v>
       </c>
-      <c r="C11" s="271"/>
+      <c r="C11" s="279"/>
       <c r="D11" s="144">
         <v>0.25</v>
       </c>
       <c r="E11" s="23">
-        <f t="shared" ref="E11:E17" si="0">D11*20</f>
+        <f>D11*20</f>
         <v>5</v>
       </c>
       <c r="F11" s="23">
-        <f t="shared" ref="F11:F17" si="1">E11*3</f>
+        <f>E11*3</f>
         <v>15</v>
       </c>
       <c r="G11" s="145">
@@ -3400,12 +3518,12 @@
         <v>0.8</v>
       </c>
       <c r="I11" s="146">
-        <f t="shared" ref="I11:I17" si="2">F11*G11*H11</f>
+        <f>F11*G11*H11</f>
         <v>360000</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B12" s="272" t="s">
+      <c r="B12" s="275" t="s">
         <v>96</v>
       </c>
       <c r="C12" s="143" t="s">
@@ -3415,11 +3533,11 @@
         <v>1.5</v>
       </c>
       <c r="E12" s="23">
-        <f t="shared" si="0"/>
+        <f>D12*20</f>
         <v>30</v>
       </c>
       <c r="F12" s="23">
-        <f t="shared" si="1"/>
+        <f>E12*3</f>
         <v>90</v>
       </c>
       <c r="G12" s="145">
@@ -3429,7 +3547,7 @@
         <v>0.8</v>
       </c>
       <c r="I12" s="146">
-        <f t="shared" si="2"/>
+        <f>F12*G12*H12</f>
         <v>2160000</v>
       </c>
       <c r="K12" s="5"/>
@@ -3446,7 +3564,7 @@
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B13" s="279"/>
+      <c r="B13" s="276"/>
       <c r="C13" s="147" t="s">
         <v>93</v>
       </c>
@@ -3454,11 +3572,11 @@
         <v>0.5</v>
       </c>
       <c r="E13" s="19">
-        <f t="shared" si="0"/>
+        <f>D13*20</f>
         <v>10</v>
       </c>
       <c r="F13" s="19">
-        <f t="shared" si="1"/>
+        <f>E13*3</f>
         <v>30</v>
       </c>
       <c r="G13" s="3">
@@ -3468,12 +3586,12 @@
         <v>0.8</v>
       </c>
       <c r="I13" s="149">
-        <f t="shared" si="2"/>
+        <f>F13*G13*H13</f>
         <v>720000</v>
       </c>
     </row>
     <row r="14" spans="2:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="274"/>
+      <c r="B14" s="277"/>
       <c r="C14" s="150" t="s">
         <v>94</v>
       </c>
@@ -3481,11 +3599,11 @@
         <v>1</v>
       </c>
       <c r="E14" s="2">
-        <f t="shared" si="0"/>
+        <f>D14*20</f>
         <v>20</v>
       </c>
       <c r="F14" s="2">
-        <f t="shared" si="1"/>
+        <f>E14*3</f>
         <v>60</v>
       </c>
       <c r="G14" s="4">
@@ -3495,12 +3613,12 @@
         <v>0.8</v>
       </c>
       <c r="I14" s="152">
-        <f t="shared" si="2"/>
+        <f>F14*G14*H14</f>
         <v>1440000</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="272" t="s">
+      <c r="B15" s="275" t="s">
         <v>98</v>
       </c>
       <c r="C15" s="143" t="s">
@@ -3510,11 +3628,11 @@
         <v>4</v>
       </c>
       <c r="E15" s="23">
-        <f t="shared" si="0"/>
+        <f>D15*20</f>
         <v>80</v>
       </c>
       <c r="F15" s="23">
-        <f t="shared" si="1"/>
+        <f>E15*3</f>
         <v>240</v>
       </c>
       <c r="G15" s="145">
@@ -3524,12 +3642,12 @@
         <v>0.8</v>
       </c>
       <c r="I15" s="146">
-        <f t="shared" si="2"/>
+        <f>F15*G15*H15</f>
         <v>5760000</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="279"/>
+      <c r="B16" s="276"/>
       <c r="C16" s="147" t="s">
         <v>93</v>
       </c>
@@ -3537,11 +3655,11 @@
         <v>0</v>
       </c>
       <c r="E16" s="19">
-        <f t="shared" si="0"/>
+        <f>D16*20</f>
         <v>0</v>
       </c>
       <c r="F16" s="19">
-        <f t="shared" si="1"/>
+        <f>E16*3</f>
         <v>0</v>
       </c>
       <c r="G16" s="3">
@@ -3551,12 +3669,12 @@
         <v>0.8</v>
       </c>
       <c r="I16" s="149">
-        <f t="shared" si="2"/>
+        <f>F16*G16*H16</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="274"/>
+      <c r="B17" s="277"/>
       <c r="C17" s="150" t="s">
         <v>94</v>
       </c>
@@ -3564,11 +3682,11 @@
         <v>0.5</v>
       </c>
       <c r="E17" s="2">
-        <f t="shared" si="0"/>
+        <f>D17*20</f>
         <v>10</v>
       </c>
       <c r="F17" s="2">
-        <f t="shared" si="1"/>
+        <f>E17*3</f>
         <v>30</v>
       </c>
       <c r="G17" s="4">
@@ -3578,7 +3696,7 @@
         <v>0.8</v>
       </c>
       <c r="I17" s="152">
-        <f t="shared" si="2"/>
+        <f>F17*G17*H17</f>
         <v>720000</v>
       </c>
     </row>
@@ -3600,28 +3718,28 @@
     </row>
     <row r="21" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B22" s="272" t="s">
+      <c r="B22" s="275" t="s">
         <v>97</v>
       </c>
       <c r="C22" s="273"/>
-      <c r="D22" s="276" t="s">
+      <c r="D22" s="270" t="s">
         <v>87</v>
       </c>
-      <c r="E22" s="276"/>
-      <c r="F22" s="276"/>
+      <c r="E22" s="270"/>
+      <c r="F22" s="270"/>
       <c r="G22" s="273" t="s">
         <v>91</v>
       </c>
       <c r="H22" s="273" t="s">
         <v>92</v>
       </c>
-      <c r="I22" s="277" t="s">
+      <c r="I22" s="271" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="23" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="274"/>
-      <c r="C23" s="275"/>
+      <c r="B23" s="277"/>
+      <c r="C23" s="274"/>
       <c r="D23" s="142" t="s">
         <v>88</v>
       </c>
@@ -3631,15 +3749,15 @@
       <c r="F23" s="142" t="s">
         <v>99</v>
       </c>
-      <c r="G23" s="275"/>
-      <c r="H23" s="275"/>
-      <c r="I23" s="278"/>
+      <c r="G23" s="274"/>
+      <c r="H23" s="274"/>
+      <c r="I23" s="272"/>
     </row>
     <row r="24" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="270" t="s">
+      <c r="B24" s="278" t="s">
         <v>100</v>
       </c>
-      <c r="C24" s="271"/>
+      <c r="C24" s="279"/>
       <c r="D24" s="153">
         <v>1</v>
       </c>
@@ -3664,28 +3782,28 @@
     </row>
     <row r="26" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="27" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B27" s="272" t="s">
+      <c r="B27" s="275" t="s">
         <v>97</v>
       </c>
       <c r="C27" s="273"/>
-      <c r="D27" s="276" t="s">
+      <c r="D27" s="270" t="s">
         <v>87</v>
       </c>
-      <c r="E27" s="276"/>
-      <c r="F27" s="276"/>
+      <c r="E27" s="270"/>
+      <c r="F27" s="270"/>
       <c r="G27" s="273" t="s">
         <v>91</v>
       </c>
       <c r="H27" s="273" t="s">
         <v>92</v>
       </c>
-      <c r="I27" s="277" t="s">
+      <c r="I27" s="271" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="28" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="274"/>
-      <c r="C28" s="275"/>
+      <c r="B28" s="277"/>
+      <c r="C28" s="274"/>
       <c r="D28" s="142" t="s">
         <v>88</v>
       </c>
@@ -3695,15 +3813,15 @@
       <c r="F28" s="142" t="s">
         <v>90</v>
       </c>
-      <c r="G28" s="275"/>
-      <c r="H28" s="275"/>
-      <c r="I28" s="278"/>
+      <c r="G28" s="274"/>
+      <c r="H28" s="274"/>
+      <c r="I28" s="272"/>
     </row>
     <row r="29" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="270" t="s">
+      <c r="B29" s="278" t="s">
         <v>101</v>
       </c>
-      <c r="C29" s="271"/>
+      <c r="C29" s="279"/>
       <c r="D29" s="153">
         <v>3</v>
       </c>
@@ -3744,12 +3862,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B9:C10"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B27:C28"/>
+    <mergeCell ref="D27:F27"/>
     <mergeCell ref="G27:G28"/>
     <mergeCell ref="H27:H28"/>
     <mergeCell ref="I27:I28"/>
@@ -3759,23 +3876,494 @@
     <mergeCell ref="G22:G23"/>
     <mergeCell ref="H22:H23"/>
     <mergeCell ref="I22:I23"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B27:C28"/>
-    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B9:C10"/>
+  </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.125" customWidth="1"/>
+    <col min="3" max="3" width="12.25" style="57" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" style="57"/>
+    <col min="11" max="11" width="11.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B1" s="57" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="H2" s="57"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B3" s="57" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="57" t="s">
+        <v>312</v>
+      </c>
+      <c r="H4" s="57" t="s">
+        <v>301</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="292" t="s">
+        <v>306</v>
+      </c>
+      <c r="D5" s="293" t="s">
+        <v>302</v>
+      </c>
+      <c r="E5" s="293" t="s">
+        <v>303</v>
+      </c>
+      <c r="F5" s="294" t="s">
+        <v>304</v>
+      </c>
+      <c r="H5" s="292" t="s">
+        <v>306</v>
+      </c>
+      <c r="I5" s="293" t="s">
+        <v>302</v>
+      </c>
+      <c r="J5" s="293" t="s">
+        <v>303</v>
+      </c>
+      <c r="K5" s="294" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C6" s="289" t="s">
+        <v>300</v>
+      </c>
+      <c r="D6" s="145">
+        <v>169</v>
+      </c>
+      <c r="E6" s="145">
+        <v>630</v>
+      </c>
+      <c r="F6" s="216">
+        <f>D6*E6</f>
+        <v>106470</v>
+      </c>
+      <c r="H6" s="289" t="s">
+        <v>300</v>
+      </c>
+      <c r="I6" s="145">
+        <v>169</v>
+      </c>
+      <c r="J6" s="145">
+        <v>500</v>
+      </c>
+      <c r="K6" s="216">
+        <f>I6*J6</f>
+        <v>84500</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C7" s="290" t="s">
+        <v>299</v>
+      </c>
+      <c r="D7" s="281">
+        <v>15</v>
+      </c>
+      <c r="E7" s="283" t="s">
+        <v>309</v>
+      </c>
+      <c r="F7" s="282">
+        <f>F6*D7/100</f>
+        <v>15970.5</v>
+      </c>
+      <c r="H7" s="290" t="s">
+        <v>299</v>
+      </c>
+      <c r="I7" s="281">
+        <v>15</v>
+      </c>
+      <c r="J7" s="283" t="s">
+        <v>309</v>
+      </c>
+      <c r="K7" s="282">
+        <f>K6*I7/100</f>
+        <v>12675</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="291" t="s">
+        <v>311</v>
+      </c>
+      <c r="D8" s="284">
+        <v>15</v>
+      </c>
+      <c r="E8" s="285" t="s">
+        <v>310</v>
+      </c>
+      <c r="F8" s="286">
+        <f>F6*D8/100</f>
+        <v>15970.5</v>
+      </c>
+      <c r="H8" s="291" t="s">
+        <v>311</v>
+      </c>
+      <c r="I8" s="284">
+        <v>0</v>
+      </c>
+      <c r="J8" s="285" t="s">
+        <v>310</v>
+      </c>
+      <c r="K8" s="286">
+        <f>K6*I8/100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" s="57" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="278" t="s">
+        <v>305</v>
+      </c>
+      <c r="D9" s="279"/>
+      <c r="E9" s="279"/>
+      <c r="F9" s="297">
+        <f>SUM(F6:F8)</f>
+        <v>138411</v>
+      </c>
+      <c r="H9" s="278" t="s">
+        <v>305</v>
+      </c>
+      <c r="I9" s="279"/>
+      <c r="J9" s="279"/>
+      <c r="K9" s="297">
+        <f>SUM(K6:K8)</f>
+        <v>97175</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C11" s="295" t="s">
+        <v>306</v>
+      </c>
+      <c r="D11" s="296" t="s">
+        <v>307</v>
+      </c>
+      <c r="E11" s="32" t="s">
+        <v>303</v>
+      </c>
+      <c r="F11" s="33" t="s">
+        <v>304</v>
+      </c>
+      <c r="H11" s="295" t="s">
+        <v>306</v>
+      </c>
+      <c r="I11" s="296" t="s">
+        <v>307</v>
+      </c>
+      <c r="J11" s="32" t="s">
+        <v>303</v>
+      </c>
+      <c r="K11" s="33" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C12" s="298" t="s">
+        <v>300</v>
+      </c>
+      <c r="D12" s="145">
+        <v>4</v>
+      </c>
+      <c r="E12" s="145">
+        <f>F9</f>
+        <v>138411</v>
+      </c>
+      <c r="F12" s="100">
+        <f>D12*E12</f>
+        <v>553644</v>
+      </c>
+      <c r="H12" s="298" t="s">
+        <v>300</v>
+      </c>
+      <c r="I12" s="145">
+        <v>4</v>
+      </c>
+      <c r="J12" s="145">
+        <f>K9</f>
+        <v>97175</v>
+      </c>
+      <c r="K12" s="100">
+        <f>I12*J12</f>
+        <v>388700</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="291" t="s">
+        <v>316</v>
+      </c>
+      <c r="D13" s="4">
+        <v>4</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0</v>
+      </c>
+      <c r="F13" s="299">
+        <f>D13*E13</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="291" t="s">
+        <v>316</v>
+      </c>
+      <c r="I13" s="4">
+        <v>4</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0</v>
+      </c>
+      <c r="K13" s="299">
+        <f>I13*J13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="278" t="s">
+        <v>308</v>
+      </c>
+      <c r="D14" s="279"/>
+      <c r="E14" s="287">
+        <f>F12</f>
+        <v>553644</v>
+      </c>
+      <c r="F14" s="288"/>
+      <c r="H14" s="278" t="s">
+        <v>308</v>
+      </c>
+      <c r="I14" s="279"/>
+      <c r="J14" s="287">
+        <f>K12</f>
+        <v>388700</v>
+      </c>
+      <c r="K14" s="288"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C15" s="280"/>
+      <c r="D15" s="280"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="3:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="3:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C18" s="292" t="s">
+        <v>306</v>
+      </c>
+      <c r="D18" s="293" t="s">
+        <v>302</v>
+      </c>
+      <c r="E18" s="293" t="s">
+        <v>303</v>
+      </c>
+      <c r="F18" s="294" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C19" s="289" t="s">
+        <v>313</v>
+      </c>
+      <c r="D19" s="145">
+        <v>37</v>
+      </c>
+      <c r="E19" s="145">
+        <v>670</v>
+      </c>
+      <c r="F19" s="216">
+        <f>D19*E19</f>
+        <v>24790</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C20" s="290" t="s">
+        <v>299</v>
+      </c>
+      <c r="D20" s="281">
+        <v>15</v>
+      </c>
+      <c r="E20" s="283" t="s">
+        <v>309</v>
+      </c>
+      <c r="F20" s="282">
+        <f>F19*D20/100</f>
+        <v>3718.5</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="291" t="s">
+        <v>311</v>
+      </c>
+      <c r="D21" s="284">
+        <v>15</v>
+      </c>
+      <c r="E21" s="285" t="s">
+        <v>310</v>
+      </c>
+      <c r="F21" s="286">
+        <f>F19*D21/100</f>
+        <v>3718.5</v>
+      </c>
+    </row>
+    <row r="22" spans="3:8" s="57" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="278" t="s">
+        <v>305</v>
+      </c>
+      <c r="D22" s="279"/>
+      <c r="E22" s="279"/>
+      <c r="F22" s="297">
+        <f>SUM(F19:F21)</f>
+        <v>32227</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="3:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C24" s="295" t="s">
+        <v>306</v>
+      </c>
+      <c r="D24" s="296" t="s">
+        <v>307</v>
+      </c>
+      <c r="E24" s="32" t="s">
+        <v>303</v>
+      </c>
+      <c r="F24" s="33" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C25" s="298" t="s">
+        <v>300</v>
+      </c>
+      <c r="D25" s="145">
+        <v>4</v>
+      </c>
+      <c r="E25" s="145">
+        <f>F22</f>
+        <v>32227</v>
+      </c>
+      <c r="F25" s="100">
+        <f>D25*E25</f>
+        <v>128908</v>
+      </c>
+    </row>
+    <row r="26" spans="3:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="291" t="s">
+        <v>314</v>
+      </c>
+      <c r="D26" s="4">
+        <v>1</v>
+      </c>
+      <c r="E26" s="4">
+        <v>110000</v>
+      </c>
+      <c r="F26" s="299">
+        <f>D26*E26</f>
+        <v>110000</v>
+      </c>
+    </row>
+    <row r="27" spans="3:8" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C27" s="291" t="s">
+        <v>316</v>
+      </c>
+      <c r="D27" s="4">
+        <v>4</v>
+      </c>
+      <c r="E27" s="4">
+        <v>0</v>
+      </c>
+      <c r="F27" s="299">
+        <f>D27*E27</f>
+        <v>0</v>
+      </c>
+      <c r="H27" s="57"/>
+    </row>
+    <row r="28" spans="3:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C28" s="278" t="s">
+        <v>308</v>
+      </c>
+      <c r="D28" s="279"/>
+      <c r="E28" s="287">
+        <f>SUM(F25:F27)</f>
+        <v>238908</v>
+      </c>
+      <c r="F28" s="288"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3958,7 +4546,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K32"/>
   <sheetViews>
@@ -4611,7 +5199,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O40"/>
   <sheetViews>
@@ -5928,7 +6516,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N56"/>
   <sheetViews>

</xml_diff>

<commit_message>
[DOC] LF GEN MCU 제작비용 update
</commit_message>
<xml_diff>
--- a/Femto Project 비용 List.xlsx
+++ b/Femto Project 비용 List.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12060" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="개발비" sheetId="7" r:id="rId1"/>
@@ -14,16 +14,17 @@
     <sheet name="0314" sheetId="8" r:id="rId5"/>
     <sheet name="0403" sheetId="10" r:id="rId6"/>
     <sheet name="0409" sheetId="12" r:id="rId7"/>
+    <sheet name="0420" sheetId="13" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4">'0314'!$B$4:$F$4</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="355">
   <si>
     <t>Vendor</t>
   </si>
@@ -47,22 +48,22 @@
   </si>
   <si>
     <t>재고</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>상품코드</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>ICbanQ</t>
   </si>
   <si>
     <t>ICbanQ</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">P002101847 </t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>NTD5802N</t>
@@ -72,11 +73,11 @@
   </si>
   <si>
     <t>53398-0471</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>50058-8000</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>CRIMP TERMINAL 51021용 (1.25mm) AWG 28,30,32</t>
@@ -89,11 +90,11 @@
   </si>
   <si>
     <t>51021-0400</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>구매수량</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>1.25mm 4-Pin Housing, Female</t>
@@ -109,90 +110,90 @@
   </si>
   <si>
     <t>Total</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>P000740132</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>P005634281</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>CTX210609-R</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>TRANSFORMER CCFL 6W 13V 11MA SMD Turn-R:100</t>
   </si>
   <si>
     <t>CTX210605-R</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>P002058985</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>P005831162</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>P002058197</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">P007073878 </t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>부가세</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>부품 Total</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>P007567011</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>NVMFS5C450NL</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>CAP TANT 220UF 16V 10% 2917</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>P008221708</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>장보고 재고 있음</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>2/5일 구매</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>T491D227K016AT</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>재고 없음</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">P007223445 </t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>2/8일 구매</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -220,19 +221,19 @@
       </rPr>
       <t>-R</t>
     </r>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>B180212004001</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>주문번호</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>2/12일 구매</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>BZT52C5V1S</t>
@@ -335,75 +336,75 @@
   </si>
   <si>
     <t>Pipette Main</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Touch Program</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>작업기간</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Month</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Day[20/Month]</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Hour[3/Day]</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>시급</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>가중치</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>LF Gen MCU</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>LF Control MCU</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Cost</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>1차 작업</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Item</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>2차 작업</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Hour[3.5/Day]</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>H/W</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>M/E</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Pipette 2차</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Set 수량</t>
@@ -413,11 +414,11 @@
   </si>
   <si>
     <t>구매 Cost</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>ICBanQ 3/14</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>STPS120M</t>
@@ -430,7 +431,7 @@
   </si>
   <si>
     <t>P001539333</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>SMBJ12CA</t>
@@ -443,15 +444,15 @@
   </si>
   <si>
     <t>P004928252</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>P007475431</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>LF용 포함 구매</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>DC-011C_SMD</t>
@@ -461,7 +462,7 @@
   </si>
   <si>
     <t>P005658771</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>053048-0310</t>
@@ -471,7 +472,7 @@
   </si>
   <si>
     <t>P005634294</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>053048-0710</t>
@@ -481,7 +482,7 @@
   </si>
   <si>
     <t>P005634298</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>HI05-AG0272</t>
@@ -494,7 +495,7 @@
   </si>
   <si>
     <t>P005659337</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>F0603E2R50FSTR</t>
@@ -507,11 +508,11 @@
   </si>
   <si>
     <t>P001574681</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>1 point 삭제 예정</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>MSS5131-153ML</t>
@@ -524,7 +525,7 @@
   </si>
   <si>
     <t xml:space="preserve">P002266417 </t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>LQM2HPZ2R2MG0</t>
@@ -537,7 +538,7 @@
   </si>
   <si>
     <t>P008172717</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>ASMT-YTD2-0BB02</t>
@@ -550,7 +551,7 @@
   </si>
   <si>
     <t>P000725384</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>17-21/W1D-ANPHY/3T</t>
@@ -563,7 +564,7 @@
   </si>
   <si>
     <t>P005609815</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>19-21/R6C-AP1Q2/3T</t>
@@ -573,7 +574,7 @@
   </si>
   <si>
     <t>P005609821</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>19-217/W1D-APQHY/3T</t>
@@ -583,11 +584,11 @@
   </si>
   <si>
     <t>P000098995</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>재품이 없어 고휘도 구매</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>19-213/G6C-AN1P2 /3T</t>
@@ -597,7 +598,7 @@
   </si>
   <si>
     <t>P005609818</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>CTT-1139P1</t>
@@ -610,11 +611,11 @@
   </si>
   <si>
     <t>P000092681</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>MOQ</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>SKRMABE010</t>
@@ -624,7 +625,7 @@
   </si>
   <si>
     <t xml:space="preserve">P001566090 </t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>STM32F070RBT6</t>
@@ -646,7 +647,7 @@
   </si>
   <si>
     <t>P000166190</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>LM2735XMF</t>
@@ -659,7 +660,7 @@
   </si>
   <si>
     <t>P006290287</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>LM3671MF-3.3</t>
@@ -669,7 +670,7 @@
   </si>
   <si>
     <t>P007302353</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>TPS3801L30</t>
@@ -679,99 +680,99 @@
   </si>
   <si>
     <t>P007092561</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>Pipette Main</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Battery 하네스</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>구매 Cost</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>ICBanQ 3/14</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>51021-0300</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>1.25mm Pitch Housing, Female, 3-Pin</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>P005634252</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>Transformer 하네스</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>51021-0700</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>1.25mm Pitch Housing, Female, 7-Pin</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>P005634256</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>50058 양단 1007 케이블</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>P005634320</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>50058 양단 케이블 L=100mm, Black</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>Date</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Cost</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Item</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Pipette Proto-type 부품 구매</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Transformer V1.0</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">Total cost : </t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Pipette V1.0 / LF MCU 일부</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Comment</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Pipette과 overlap되는 LF MCU 부품 구매</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>ON Semiconductor</t>
@@ -784,478 +785,478 @@
   </si>
   <si>
     <t>구매수량</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Total</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>재고</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>주문번호</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>EX-936ESD</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve"> EXSO </t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>정전기 방지 온도조절형 인두, 소비전력:60W, 온도:220℃ ~ 480℃</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>P001909039</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">LedSol 3001 </t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>EXSO</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>디지털 무연인두기, 75W, 온도: 100~500℃</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>P007193509</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">LedSol-100 </t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>아날로그 무연인두기 , 24V 75W, 온도: 200~480℃</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>P007193511</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">LedSol-200 </t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>디지털 무연인두기, 24V 70W, 온도: 200~480℃</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>P007193512</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>FX-888D(70W)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>HAKKO</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>디지털 무연인두기, 26V 70W, 온도: 200~480℃</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>P005688453</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>FX-951</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>디지털 무연인두기, 24V 75W, 온도: 200~450℃</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>P005688454</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>T18-K</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>HAKKO</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>HAKKO FX-888(FX-8801) 전용 인두 칼팁</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>P002116124</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>T18-3.5K</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>T18-B</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>HAKKO FX-888(FX-8801) 전용 인두 팁</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">P002116123 </t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>B3474</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Rubber Cleaner</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>A1561</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>HAKKO A1561 클리닝와이어</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>P004702618</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>A1559</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>HAKKO A1559 스폰지</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>P004704819</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>SPPON 18</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>HAKKO 18 SPPON DESOLDERING TOOL</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>P004702809</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>18N.18G</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>HAKKO SPPON NOZZLE</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>ic114</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>UL1007-AWG20</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>UL전선</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>극세선 난연성 전선(UL전선) / AWG20 / 길이(30M) (검정색)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">P002329495 </t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>극세선 난연성 전선(UL전선) / AWG20 / 길이(30M) (빨강)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">P002329190 </t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>칩저항 키트</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Any vender</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>1005 사이즈 F급(1%) 160종 칩저항 키트 - (100개들이)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>P001907055</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>JL-0232 적색</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Any vender</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">더블 바나나플러그 / 적색 </t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>P005658758</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>GHG630DCE</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve"> BOSCH </t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>열풍기(히터건) (GHG630DCE)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>P007320842</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>ST-LINK/V2</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>STMicroelectronics</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>ICD/PROGRAMMER, FOR STM8, STM32</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>P001648331</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>ENGINEER SL-04</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>ENGINEER SL-04 DESK-TOP LOUPE, 렌즈 직경 75mm, 배율 3X</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">P004704041 </t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>8611L</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>8611L LED조명 확대경, 렌즈 직경 89mm, 배율 3X</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>P004704064</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>824-22-003-00-005000</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Mill-Max</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">Mill-Max Pin &amp; Socket Connectors </t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>P008110102</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Transformer PCB</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>재고</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>ICBanQ 3/14</t>
   </si>
   <si>
     <t>P007567011</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>P005634282</t>
-    <phoneticPr fontId="32" type="noConversion"/>
+    <phoneticPr fontId="33" type="noConversion"/>
   </si>
   <si>
     <t>재고 소진</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Pipette V1.0 부품 및 장비</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>실험실에서 사용할 장비 및 Pipette 관련 추가 부품</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>부자재</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>수삽</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>개인</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Point</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>단가</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>금액</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>소계</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>작업내용</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>수량</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>합계</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>-</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>-</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>이윤</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>SMD</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Metal mask</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Sample용 견적</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>부품비</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>LF Generator MCU Board</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">HIPPO 6구 접지 멀티탭 멀티탭 - 기본 1.5M </t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">HIPPO 6구 접지 멀티탭 멀티탭 - 3M </t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>HIPPO</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>KFT HT-5023 스트리퍼 (AWG20~30)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">KFT </t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>P001415029</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>페이스트 [135-0805]</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>P008012287</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>정전기매트 120cm*1M</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>P000119604</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">P007311227 </t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>실험실 물품 구매</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>제이엘텍 - Sample build 견적</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>LF GEN MCU 부품 구매</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>HEADER_2.54mm_2x5</t>
@@ -1322,18 +1323,26 @@
   </si>
   <si>
     <t>Exso</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>40V, 2.8mOhm , 110A, Single N−Channel Power MOSFET</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>PCB Artwork</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total</t>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="7">
+  <numFmts count="9">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;?_-;_-@_-"/>
@@ -1341,13 +1350,23 @@
     <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="0.0"/>
     <numFmt numFmtId="180" formatCode="0\ &quot;%&quot;"/>
+    <numFmt numFmtId="183" formatCode="0.0\ &quot;ea&quot;"/>
+    <numFmt numFmtId="184" formatCode="0.0\ &quot;일&quot;"/>
   </numFmts>
-  <fonts count="33" x14ac:knownFonts="1">
+  <fonts count="34" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2274,287 +2293,287 @@
   </borders>
   <cellStyleXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="311">
+  <cellXfs count="317">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
@@ -2569,7 +2588,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="43" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="43" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2578,7 +2597,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="43" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="43" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2593,32 +2612,32 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="27" fillId="33" borderId="11" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="28" fillId="33" borderId="11" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="43" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="27" fillId="33" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="43" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="33" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="43" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="43" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="43" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="43" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="43" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="43" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="43" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="43" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="52" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="52" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2632,21 +2651,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="52" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="52" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="52" applyFill="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="41" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="41" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="176" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2659,26 +2678,26 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="27" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="28" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="36" borderId="16" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="16" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="36" borderId="17" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="17" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="36" borderId="17" xfId="43" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="17" xfId="43" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2691,13 +2710,13 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="43" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="43" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -2710,16 +2729,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="28" fillId="34" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="41" fontId="29" fillId="34" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="41" fontId="0" fillId="34" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="41" fontId="0" fillId="34" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="33" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="33" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="33" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="33" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -2766,34 +2785,34 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="41" fontId="0" fillId="34" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="41" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="27" fillId="33" borderId="24" xfId="69" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="28" fillId="33" borderId="24" xfId="69" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="35" borderId="25" xfId="69" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="35" borderId="25" xfId="69" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="69" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="27" fillId="33" borderId="11" xfId="69" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="69" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="33" borderId="11" xfId="69" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="35" borderId="12" xfId="69" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="35" borderId="12" xfId="69" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="69" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="69" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="69" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="69" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="69" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="69" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2816,68 +2835,68 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="75" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="75" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="75" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="75" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="75">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="75" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="75">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="75" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="27" fillId="0" borderId="0" xfId="75" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="27" fillId="33" borderId="23" xfId="75" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="0" xfId="75" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="33" borderId="23" xfId="75" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="27" fillId="33" borderId="24" xfId="75" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="28" fillId="33" borderId="24" xfId="75" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="27" fillId="33" borderId="33" xfId="75" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="28" fillId="33" borderId="33" xfId="75" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="27" fillId="33" borderId="23" xfId="69" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="28" fillId="33" borderId="23" xfId="69" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="75" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="75" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="75" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="75" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="75" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="75" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="27" xfId="76" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="75" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="75" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="75" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="75" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="75" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="75" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="26" xfId="76" applyFont="1" applyBorder="1">
@@ -2889,46 +2908,46 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="14" xfId="76" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="15" xfId="75" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="15" xfId="75" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="16" xfId="76" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="69" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="69" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="17" xfId="76" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="18" xfId="75" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="17" xfId="75" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="17" xfId="75" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="18" xfId="75" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="17" xfId="75" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="17" xfId="75" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="26" xfId="76" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="18" xfId="69" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="27" fillId="0" borderId="22" xfId="76" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" xfId="75" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="75" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="18" xfId="69" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="28" fillId="0" borderId="22" xfId="76" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" xfId="75" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="75" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2937,7 +2956,7 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="27" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="28" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2983,23 +3002,23 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="41" fontId="27" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="41" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="27" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="28" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="27" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="28" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="41" fontId="27" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="28" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -3017,125 +3036,125 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="27" fillId="33" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="33" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="27" fillId="33" borderId="23" xfId="77" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="28" fillId="33" borderId="23" xfId="77" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="27" fillId="33" borderId="24" xfId="77" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="28" fillId="33" borderId="24" xfId="77" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="77" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="77" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="77" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="77" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="77" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="77" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="37" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="27" fillId="33" borderId="10" xfId="78" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="28" fillId="33" borderId="10" xfId="78" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="27" fillId="33" borderId="11" xfId="78" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="28" fillId="33" borderId="11" xfId="78" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="78" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="78" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="78">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="78" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="78" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="78">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="37" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="78" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="34" borderId="25" xfId="69" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="78" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="25" xfId="69" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="78" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="78" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="78" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="27" fillId="33" borderId="24" xfId="78" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="78" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="33" borderId="24" xfId="78" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="78" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="78" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="78" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="14" xfId="79" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="78" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="78" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="14" xfId="79" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="78" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="78" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="78" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="17" xfId="79" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="78" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="78" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="78" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="17" xfId="79" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="78" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="78" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="78" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="20" xfId="79" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="20" xfId="79" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="78" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="78" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" xfId="79" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="78" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="14" xfId="79" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="15" xfId="78" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="78" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="17" xfId="79" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="78" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="78" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="78" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="20" xfId="79" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="20" xfId="79" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="78" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="78" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" xfId="79" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="78" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="14" xfId="79" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="15" xfId="78" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="78" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="17" xfId="79" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="78" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -3148,112 +3167,122 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="27" fillId="33" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="28" fillId="33" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="27" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="41" fontId="28" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="80" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="17" xfId="80" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="80" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="17" xfId="80" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="80" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="80" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="80" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="17" xfId="95" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="80" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="17" xfId="80" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="80" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="17" xfId="80" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="80" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="80" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="80" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="17" xfId="95" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="15" xfId="78" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="18" xfId="80" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="21" xfId="78" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="18" xfId="78" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="43" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="27" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="28" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="41" fontId="27" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="28" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="34" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="34" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="34" borderId="15" xfId="78" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="34" borderId="18" xfId="80" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="34" borderId="21" xfId="78" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="34" borderId="18" xfId="78" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="34" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="34" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="43" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="183" fontId="0" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="184" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="28" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="28" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="96">
     <cellStyle name="20% - 강조색1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3409,7 +3438,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3444,7 +3473,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3656,7 +3685,7 @@
   <dimension ref="B6:O34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3681,28 +3710,28 @@
     </row>
     <row r="8" spans="2:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="291" t="s">
+      <c r="B9" s="303" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="292"/>
-      <c r="D9" s="295" t="s">
+      <c r="C9" s="301"/>
+      <c r="D9" s="298" t="s">
         <v>86</v>
       </c>
-      <c r="E9" s="295"/>
-      <c r="F9" s="295"/>
-      <c r="G9" s="292" t="s">
+      <c r="E9" s="298"/>
+      <c r="F9" s="298"/>
+      <c r="G9" s="301" t="s">
         <v>90</v>
       </c>
-      <c r="H9" s="292" t="s">
+      <c r="H9" s="301" t="s">
         <v>91</v>
       </c>
-      <c r="I9" s="296" t="s">
+      <c r="I9" s="299" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="10" spans="2:14" s="138" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="293"/>
-      <c r="C10" s="294"/>
+      <c r="B10" s="305"/>
+      <c r="C10" s="302"/>
       <c r="D10" s="139" t="s">
         <v>87</v>
       </c>
@@ -3712,15 +3741,15 @@
       <c r="F10" s="139" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="294"/>
-      <c r="H10" s="294"/>
-      <c r="I10" s="297"/>
+      <c r="G10" s="302"/>
+      <c r="H10" s="302"/>
+      <c r="I10" s="300"/>
     </row>
     <row r="11" spans="2:14" s="138" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="289" t="s">
+      <c r="B11" s="306" t="s">
         <v>101</v>
       </c>
-      <c r="C11" s="290"/>
+      <c r="C11" s="307"/>
       <c r="D11" s="141">
         <v>0.25</v>
       </c>
@@ -3744,7 +3773,7 @@
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B12" s="291" t="s">
+      <c r="B12" s="303" t="s">
         <v>95</v>
       </c>
       <c r="C12" s="140" t="s">
@@ -3785,7 +3814,7 @@
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B13" s="298"/>
+      <c r="B13" s="304"/>
       <c r="C13" s="144" t="s">
         <v>92</v>
       </c>
@@ -3812,7 +3841,7 @@
       </c>
     </row>
     <row r="14" spans="2:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="293"/>
+      <c r="B14" s="305"/>
       <c r="C14" s="147" t="s">
         <v>93</v>
       </c>
@@ -3839,7 +3868,7 @@
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="291" t="s">
+      <c r="B15" s="303" t="s">
         <v>97</v>
       </c>
       <c r="C15" s="140" t="s">
@@ -3868,7 +3897,7 @@
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="298"/>
+      <c r="B16" s="304"/>
       <c r="C16" s="144" t="s">
         <v>92</v>
       </c>
@@ -3895,7 +3924,7 @@
       </c>
     </row>
     <row r="17" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="293"/>
+      <c r="B17" s="305"/>
       <c r="C17" s="147" t="s">
         <v>93</v>
       </c>
@@ -3939,28 +3968,28 @@
     </row>
     <row r="21" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B22" s="291" t="s">
+      <c r="B22" s="303" t="s">
         <v>96</v>
       </c>
-      <c r="C22" s="292"/>
-      <c r="D22" s="295" t="s">
+      <c r="C22" s="301"/>
+      <c r="D22" s="298" t="s">
         <v>86</v>
       </c>
-      <c r="E22" s="295"/>
-      <c r="F22" s="295"/>
-      <c r="G22" s="292" t="s">
+      <c r="E22" s="298"/>
+      <c r="F22" s="298"/>
+      <c r="G22" s="301" t="s">
         <v>90</v>
       </c>
-      <c r="H22" s="292" t="s">
+      <c r="H22" s="301" t="s">
         <v>91</v>
       </c>
-      <c r="I22" s="296" t="s">
+      <c r="I22" s="299" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="23" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="293"/>
-      <c r="C23" s="294"/>
+      <c r="B23" s="305"/>
+      <c r="C23" s="302"/>
       <c r="D23" s="139" t="s">
         <v>87</v>
       </c>
@@ -3970,15 +3999,15 @@
       <c r="F23" s="139" t="s">
         <v>98</v>
       </c>
-      <c r="G23" s="294"/>
-      <c r="H23" s="294"/>
-      <c r="I23" s="297"/>
+      <c r="G23" s="302"/>
+      <c r="H23" s="302"/>
+      <c r="I23" s="300"/>
     </row>
     <row r="24" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="289" t="s">
+      <c r="B24" s="306" t="s">
         <v>99</v>
       </c>
-      <c r="C24" s="290"/>
+      <c r="C24" s="307"/>
       <c r="D24" s="150">
         <v>1</v>
       </c>
@@ -4003,28 +4032,28 @@
     </row>
     <row r="26" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="27" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B27" s="291" t="s">
+      <c r="B27" s="303" t="s">
         <v>96</v>
       </c>
-      <c r="C27" s="292"/>
-      <c r="D27" s="295" t="s">
+      <c r="C27" s="301"/>
+      <c r="D27" s="298" t="s">
         <v>86</v>
       </c>
-      <c r="E27" s="295"/>
-      <c r="F27" s="295"/>
-      <c r="G27" s="292" t="s">
+      <c r="E27" s="298"/>
+      <c r="F27" s="298"/>
+      <c r="G27" s="301" t="s">
         <v>90</v>
       </c>
-      <c r="H27" s="292" t="s">
+      <c r="H27" s="301" t="s">
         <v>91</v>
       </c>
-      <c r="I27" s="296" t="s">
+      <c r="I27" s="299" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="28" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="293"/>
-      <c r="C28" s="294"/>
+      <c r="B28" s="305"/>
+      <c r="C28" s="302"/>
       <c r="D28" s="139" t="s">
         <v>87</v>
       </c>
@@ -4034,15 +4063,15 @@
       <c r="F28" s="139" t="s">
         <v>89</v>
       </c>
-      <c r="G28" s="294"/>
-      <c r="H28" s="294"/>
-      <c r="I28" s="297"/>
+      <c r="G28" s="302"/>
+      <c r="H28" s="302"/>
+      <c r="I28" s="300"/>
     </row>
     <row r="29" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="289" t="s">
+      <c r="B29" s="306" t="s">
         <v>100</v>
       </c>
-      <c r="C29" s="290"/>
+      <c r="C29" s="307"/>
       <c r="D29" s="150">
         <v>3</v>
       </c>
@@ -4083,12 +4112,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B9:C10"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B27:C28"/>
+    <mergeCell ref="D27:F27"/>
     <mergeCell ref="G27:G28"/>
     <mergeCell ref="H27:H28"/>
     <mergeCell ref="I27:I28"/>
@@ -4098,13 +4126,14 @@
     <mergeCell ref="G22:G23"/>
     <mergeCell ref="H22:H23"/>
     <mergeCell ref="I22:I23"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B27:C28"/>
-    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B9:C10"/>
   </mergeCells>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4115,7 +4144,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="N4" sqref="N4:S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4128,6 +4157,7 @@
     <col min="6" max="6" width="10.875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="56"/>
     <col min="11" max="11" width="11.5" customWidth="1"/>
+    <col min="17" max="17" width="9.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.3">
@@ -4203,11 +4233,11 @@
         <v>169</v>
       </c>
       <c r="J6" s="142">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="K6" s="213">
         <f>I6*J6</f>
-        <v>84500</v>
+        <v>42250</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
@@ -4228,14 +4258,14 @@
         <v>298</v>
       </c>
       <c r="I7" s="263">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="J7" s="265" t="s">
         <v>308</v>
       </c>
       <c r="K7" s="264">
         <f>K6*I7/100</f>
-        <v>12675</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -4267,23 +4297,23 @@
       </c>
     </row>
     <row r="9" spans="2:11" s="56" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="289" t="s">
+      <c r="C9" s="306" t="s">
         <v>304</v>
       </c>
-      <c r="D9" s="290"/>
-      <c r="E9" s="290"/>
+      <c r="D9" s="307"/>
+      <c r="E9" s="307"/>
       <c r="F9" s="277">
         <f>SUM(F6:F8)</f>
         <v>138411</v>
       </c>
-      <c r="H9" s="289" t="s">
+      <c r="H9" s="306" t="s">
         <v>304</v>
       </c>
-      <c r="I9" s="290"/>
-      <c r="J9" s="290"/>
+      <c r="I9" s="307"/>
+      <c r="J9" s="307"/>
       <c r="K9" s="277">
         <f>SUM(K6:K8)</f>
-        <v>97175</v>
+        <v>42250</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -4343,11 +4373,11 @@
       </c>
       <c r="J12" s="142">
         <f>K9</f>
-        <v>97175</v>
+        <v>42250</v>
       </c>
       <c r="K12" s="99">
         <f>I12*J12</f>
-        <v>388700</v>
+        <v>169000</v>
       </c>
     </row>
     <row r="13" spans="2:11" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -4379,28 +4409,28 @@
       </c>
     </row>
     <row r="14" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="289" t="s">
+      <c r="C14" s="306" t="s">
         <v>307</v>
       </c>
-      <c r="D14" s="290"/>
-      <c r="E14" s="299">
+      <c r="D14" s="307"/>
+      <c r="E14" s="308">
         <f>F12</f>
         <v>553644</v>
       </c>
-      <c r="F14" s="300"/>
-      <c r="H14" s="289" t="s">
+      <c r="F14" s="309"/>
+      <c r="H14" s="306" t="s">
         <v>307</v>
       </c>
-      <c r="I14" s="290"/>
-      <c r="J14" s="299">
+      <c r="I14" s="307"/>
+      <c r="J14" s="308">
         <f>K12</f>
-        <v>388700</v>
-      </c>
-      <c r="K14" s="300"/>
+        <v>169000</v>
+      </c>
+      <c r="K14" s="309"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C15" s="301"/>
-      <c r="D15" s="301"/>
+      <c r="C15" s="310"/>
+      <c r="D15" s="310"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
@@ -4474,11 +4504,11 @@
       </c>
     </row>
     <row r="22" spans="3:8" s="56" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="289" t="s">
+      <c r="C22" s="306" t="s">
         <v>304</v>
       </c>
-      <c r="D22" s="290"/>
-      <c r="E22" s="290"/>
+      <c r="D22" s="307"/>
+      <c r="E22" s="307"/>
       <c r="F22" s="277">
         <f>SUM(F19:F21)</f>
         <v>45292</v>
@@ -4551,15 +4581,15 @@
       <c r="H27" s="56"/>
     </row>
     <row r="28" spans="3:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C28" s="289" t="s">
+      <c r="C28" s="306" t="s">
         <v>307</v>
       </c>
-      <c r="D28" s="290"/>
-      <c r="E28" s="299">
+      <c r="D28" s="307"/>
+      <c r="E28" s="308">
         <f>SUM(F25:F27)</f>
         <v>291168</v>
       </c>
-      <c r="F28" s="300"/>
+      <c r="F28" s="309"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -4574,7 +4604,7 @@
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C15:D15"/>
   </mergeCells>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4762,7 +4792,7 @@
       <c r="E22" s="218"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
@@ -4895,7 +4925,7 @@
       <c r="C6" s="22">
         <v>2</v>
       </c>
-      <c r="D6" s="310" t="s">
+      <c r="D6" s="297" t="s">
         <v>352</v>
       </c>
       <c r="E6" s="53" t="s">
@@ -5415,7 +5445,7 @@
       <c r="K32" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
@@ -6732,7 +6762,7 @@
     </row>
   </sheetData>
   <autoFilter ref="B4:F4"/>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -6742,7 +6772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
@@ -7081,7 +7111,7 @@
         <v>13000</v>
       </c>
       <c r="K11" s="17"/>
-      <c r="L11" s="302" t="s">
+      <c r="L11" s="289" t="s">
         <v>243</v>
       </c>
     </row>
@@ -7134,7 +7164,7 @@
         <v>8000</v>
       </c>
       <c r="K13" s="17"/>
-      <c r="L13" s="302" t="s">
+      <c r="L13" s="289" t="s">
         <v>248</v>
       </c>
     </row>
@@ -7168,7 +7198,7 @@
         <v>9000</v>
       </c>
       <c r="K14" s="17"/>
-      <c r="L14" s="302" t="s">
+      <c r="L14" s="289" t="s">
         <v>251</v>
       </c>
     </row>
@@ -7202,7 +7232,7 @@
         <v>16500</v>
       </c>
       <c r="K15" s="17"/>
-      <c r="L15" s="302" t="s">
+      <c r="L15" s="289" t="s">
         <v>254</v>
       </c>
     </row>
@@ -7261,7 +7291,7 @@
         <v>9000</v>
       </c>
       <c r="K17" s="17"/>
-      <c r="L17" s="302" t="s">
+      <c r="L17" s="289" t="s">
         <v>261</v>
       </c>
     </row>
@@ -7295,7 +7325,7 @@
         <v>9000</v>
       </c>
       <c r="K18" s="17"/>
-      <c r="L18" s="302" t="s">
+      <c r="L18" s="289" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7329,7 +7359,7 @@
         <v>180000</v>
       </c>
       <c r="K19" s="108"/>
-      <c r="L19" s="303" t="s">
+      <c r="L19" s="290" t="s">
         <v>267</v>
       </c>
     </row>
@@ -7363,7 +7393,7 @@
         <v>2420</v>
       </c>
       <c r="K20" s="108"/>
-      <c r="L20" s="303" t="s">
+      <c r="L20" s="290" t="s">
         <v>271</v>
       </c>
     </row>
@@ -7397,7 +7427,7 @@
         <v>101200</v>
       </c>
       <c r="K21" s="108"/>
-      <c r="L21" s="303" t="s">
+      <c r="L21" s="290" t="s">
         <v>275</v>
       </c>
     </row>
@@ -7431,7 +7461,7 @@
         <v>49000</v>
       </c>
       <c r="K22" s="108"/>
-      <c r="L22" s="303" t="s">
+      <c r="L22" s="290" t="s">
         <v>279</v>
       </c>
     </row>
@@ -7488,7 +7518,7 @@
         <v>45000</v>
       </c>
       <c r="K24" s="103"/>
-      <c r="L24" s="309" t="s">
+      <c r="L24" s="296" t="s">
         <v>285</v>
       </c>
     </row>
@@ -7581,7 +7611,7 @@
         <v>7200</v>
       </c>
       <c r="K31" s="35"/>
-      <c r="L31" s="304" t="s">
+      <c r="L31" s="291" t="s">
         <v>54</v>
       </c>
       <c r="M31" s="232" t="s">
@@ -7618,7 +7648,7 @@
         <v>7040</v>
       </c>
       <c r="K32" s="36"/>
-      <c r="L32" s="306" t="s">
+      <c r="L32" s="293" t="s">
         <v>289</v>
       </c>
     </row>
@@ -7670,7 +7700,7 @@
       <c r="C37" s="189" t="s">
         <v>208</v>
       </c>
-      <c r="D37" s="310" t="s">
+      <c r="D37" s="297" t="s">
         <v>352</v>
       </c>
       <c r="E37" s="35" t="s">
@@ -7727,7 +7757,7 @@
         <v>13000</v>
       </c>
       <c r="K38" s="36"/>
-      <c r="L38" s="308" t="s">
+      <c r="L38" s="295" t="s">
         <v>294</v>
       </c>
     </row>
@@ -7814,7 +7844,7 @@
         <v>10500</v>
       </c>
       <c r="K43" s="35"/>
-      <c r="L43" s="304" t="s">
+      <c r="L43" s="291" t="s">
         <v>67</v>
       </c>
     </row>
@@ -7847,7 +7877,7 @@
         <v>2100</v>
       </c>
       <c r="K44" s="105"/>
-      <c r="L44" s="307" t="s">
+      <c r="L44" s="294" t="s">
         <v>70</v>
       </c>
     </row>
@@ -7878,7 +7908,7 @@
         <v>4000</v>
       </c>
       <c r="K45" s="36"/>
-      <c r="L45" s="306" t="s">
+      <c r="L45" s="293" t="s">
         <v>73</v>
       </c>
     </row>
@@ -8002,7 +8032,7 @@
         <v>2000</v>
       </c>
       <c r="K50" s="105"/>
-      <c r="L50" s="307" t="s">
+      <c r="L50" s="294" t="s">
         <v>81</v>
       </c>
     </row>
@@ -8035,7 +8065,7 @@
         <v>2000</v>
       </c>
       <c r="K51" s="36"/>
-      <c r="L51" s="306" t="s">
+      <c r="L51" s="293" t="s">
         <v>83</v>
       </c>
     </row>
@@ -8064,7 +8094,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
@@ -8153,7 +8183,7 @@
         <v>6000</v>
       </c>
       <c r="K4" s="19"/>
-      <c r="L4" s="302" t="s">
+      <c r="L4" s="289" t="s">
         <v>326</v>
       </c>
     </row>
@@ -8183,7 +8213,7 @@
         <v>8000</v>
       </c>
       <c r="K5" s="19"/>
-      <c r="L5" s="302" t="s">
+      <c r="L5" s="289" t="s">
         <v>326</v>
       </c>
     </row>
@@ -8213,7 +8243,7 @@
         <v>7000</v>
       </c>
       <c r="K6" s="19"/>
-      <c r="L6" s="302" t="s">
+      <c r="L6" s="289" t="s">
         <v>321</v>
       </c>
     </row>
@@ -8243,7 +8273,7 @@
         <v>2600</v>
       </c>
       <c r="K7" s="19"/>
-      <c r="L7" s="302" t="s">
+      <c r="L7" s="289" t="s">
         <v>323</v>
       </c>
     </row>
@@ -8271,7 +8301,7 @@
         <v>44000</v>
       </c>
       <c r="K8" s="19"/>
-      <c r="L8" s="302" t="s">
+      <c r="L8" s="289" t="s">
         <v>325</v>
       </c>
     </row>
@@ -8428,7 +8458,7 @@
         <v>300</v>
       </c>
       <c r="K20" s="19"/>
-      <c r="L20" s="305" t="s">
+      <c r="L20" s="292" t="s">
         <v>345</v>
       </c>
     </row>
@@ -8462,7 +8492,7 @@
         <v>5000</v>
       </c>
       <c r="K21" s="19"/>
-      <c r="L21" s="305" t="s">
+      <c r="L21" s="292" t="s">
         <v>346</v>
       </c>
     </row>
@@ -8496,7 +8526,7 @@
         <v>5800</v>
       </c>
       <c r="K22" s="19"/>
-      <c r="L22" s="305" t="s">
+      <c r="L22" s="292" t="s">
         <v>347</v>
       </c>
     </row>
@@ -8530,7 +8560,7 @@
         <v>1000</v>
       </c>
       <c r="K23" s="19"/>
-      <c r="L23" s="305" t="s">
+      <c r="L23" s="292" t="s">
         <v>348</v>
       </c>
     </row>
@@ -8564,7 +8594,7 @@
         <v>4300</v>
       </c>
       <c r="K24" s="19"/>
-      <c r="L24" s="305" t="s">
+      <c r="L24" s="292" t="s">
         <v>349</v>
       </c>
     </row>
@@ -8598,7 +8628,7 @@
         <v>4300</v>
       </c>
       <c r="K25" s="19"/>
-      <c r="L25" s="305" t="s">
+      <c r="L25" s="292" t="s">
         <v>350</v>
       </c>
     </row>
@@ -8627,8 +8657,125 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="56" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C3" s="272" t="s">
+        <v>305</v>
+      </c>
+      <c r="D3" s="273" t="s">
+        <v>301</v>
+      </c>
+      <c r="E3" s="273" t="s">
+        <v>302</v>
+      </c>
+      <c r="F3" s="274" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="315" t="s">
+        <v>299</v>
+      </c>
+      <c r="D4" s="151">
+        <v>169</v>
+      </c>
+      <c r="E4" s="151">
+        <v>250</v>
+      </c>
+      <c r="F4" s="316">
+        <f>D4*E4</f>
+        <v>42250</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="275" t="s">
+        <v>305</v>
+      </c>
+      <c r="D6" s="276" t="s">
+        <v>306</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>302</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="56"/>
+      <c r="C7" s="278" t="s">
+        <v>299</v>
+      </c>
+      <c r="D7" s="311">
+        <v>3</v>
+      </c>
+      <c r="E7" s="142">
+        <v>40000</v>
+      </c>
+      <c r="F7" s="213">
+        <f>D7*E7</f>
+        <v>120000</v>
+      </c>
+      <c r="G7" s="56"/>
+    </row>
+    <row r="8" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="233" t="s">
+        <v>353</v>
+      </c>
+      <c r="D8" s="312">
+        <v>2</v>
+      </c>
+      <c r="E8" s="4">
+        <v>250000</v>
+      </c>
+      <c r="F8" s="219">
+        <f>D8*E8</f>
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="306" t="s">
+        <v>354</v>
+      </c>
+      <c r="D9" s="307"/>
+      <c r="E9" s="313">
+        <f>SUM(F7:F8)</f>
+        <v>620000</v>
+      </c>
+      <c r="F9" s="314"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="C9:D9"/>
+  </mergeCells>
+  <phoneticPr fontId="10" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[DOC] 구매 부품 list update and Sample  대장 update
</commit_message>
<xml_diff>
--- a/Femto Project 비용 List.xlsx
+++ b/Femto Project 비용 List.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12060" activeTab="7"/>
@@ -15,16 +15,17 @@
     <sheet name="0403" sheetId="10" r:id="rId6"/>
     <sheet name="0409" sheetId="12" r:id="rId7"/>
     <sheet name="0420" sheetId="13" r:id="rId8"/>
+    <sheet name="부품 list" sheetId="14" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4">'0314'!$B$4:$F$4</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="359">
   <si>
     <t>Vendor</t>
   </si>
@@ -1337,6 +1338,22 @@
     <t>Total</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
+  <si>
+    <t>Transformer</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pipette Main</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>LF MCU</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -1350,8 +1367,8 @@
     <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="0.0"/>
     <numFmt numFmtId="180" formatCode="0\ &quot;%&quot;"/>
-    <numFmt numFmtId="183" formatCode="0.0\ &quot;ea&quot;"/>
-    <numFmt numFmtId="184" formatCode="0.0\ &quot;일&quot;"/>
+    <numFmt numFmtId="181" formatCode="0.0\ &quot;ea&quot;"/>
+    <numFmt numFmtId="182" formatCode="0.0\ &quot;일&quot;"/>
   </numFmts>
   <fonts count="34" x14ac:knownFonts="1">
     <font>
@@ -1843,7 +1860,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -2290,6 +2307,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2573,7 +2614,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="317">
+  <cellXfs count="369">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
@@ -3234,6 +3275,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="43" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3243,27 +3309,9 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="41" fontId="28" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3273,16 +3321,165 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="183" fontId="0" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="184" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="28" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="41" fontId="28" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="28" fillId="33" borderId="34" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="28" fillId="33" borderId="35" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="78" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="43" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="52" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="75" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="75" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="75" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="75" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="75" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="75" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="69" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="78" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="43" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="78" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="80" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="80" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="80" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="80" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="80" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="20" xfId="80" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="29" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="96">
     <cellStyle name="20% - 강조색1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3438,7 +3635,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3473,7 +3670,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3710,28 +3907,28 @@
     </row>
     <row r="8" spans="2:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="303" t="s">
+      <c r="B9" s="305" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="301"/>
-      <c r="D9" s="298" t="s">
+      <c r="C9" s="306"/>
+      <c r="D9" s="309" t="s">
         <v>86</v>
       </c>
-      <c r="E9" s="298"/>
-      <c r="F9" s="298"/>
-      <c r="G9" s="301" t="s">
+      <c r="E9" s="309"/>
+      <c r="F9" s="309"/>
+      <c r="G9" s="306" t="s">
         <v>90</v>
       </c>
-      <c r="H9" s="301" t="s">
+      <c r="H9" s="306" t="s">
         <v>91</v>
       </c>
-      <c r="I9" s="299" t="s">
+      <c r="I9" s="310" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="10" spans="2:14" s="138" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="305"/>
-      <c r="C10" s="302"/>
+      <c r="B10" s="307"/>
+      <c r="C10" s="308"/>
       <c r="D10" s="139" t="s">
         <v>87</v>
       </c>
@@ -3741,15 +3938,15 @@
       <c r="F10" s="139" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="302"/>
-      <c r="H10" s="302"/>
-      <c r="I10" s="300"/>
+      <c r="G10" s="308"/>
+      <c r="H10" s="308"/>
+      <c r="I10" s="311"/>
     </row>
     <row r="11" spans="2:14" s="138" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="306" t="s">
+      <c r="B11" s="303" t="s">
         <v>101</v>
       </c>
-      <c r="C11" s="307"/>
+      <c r="C11" s="304"/>
       <c r="D11" s="141">
         <v>0.25</v>
       </c>
@@ -3773,7 +3970,7 @@
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B12" s="303" t="s">
+      <c r="B12" s="305" t="s">
         <v>95</v>
       </c>
       <c r="C12" s="140" t="s">
@@ -3814,7 +4011,7 @@
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B13" s="304"/>
+      <c r="B13" s="312"/>
       <c r="C13" s="144" t="s">
         <v>92</v>
       </c>
@@ -3841,7 +4038,7 @@
       </c>
     </row>
     <row r="14" spans="2:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="305"/>
+      <c r="B14" s="307"/>
       <c r="C14" s="147" t="s">
         <v>93</v>
       </c>
@@ -3868,7 +4065,7 @@
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="303" t="s">
+      <c r="B15" s="305" t="s">
         <v>97</v>
       </c>
       <c r="C15" s="140" t="s">
@@ -3897,7 +4094,7 @@
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="304"/>
+      <c r="B16" s="312"/>
       <c r="C16" s="144" t="s">
         <v>92</v>
       </c>
@@ -3924,7 +4121,7 @@
       </c>
     </row>
     <row r="17" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="305"/>
+      <c r="B17" s="307"/>
       <c r="C17" s="147" t="s">
         <v>93</v>
       </c>
@@ -3968,28 +4165,28 @@
     </row>
     <row r="21" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B22" s="303" t="s">
+      <c r="B22" s="305" t="s">
         <v>96</v>
       </c>
-      <c r="C22" s="301"/>
-      <c r="D22" s="298" t="s">
+      <c r="C22" s="306"/>
+      <c r="D22" s="309" t="s">
         <v>86</v>
       </c>
-      <c r="E22" s="298"/>
-      <c r="F22" s="298"/>
-      <c r="G22" s="301" t="s">
+      <c r="E22" s="309"/>
+      <c r="F22" s="309"/>
+      <c r="G22" s="306" t="s">
         <v>90</v>
       </c>
-      <c r="H22" s="301" t="s">
+      <c r="H22" s="306" t="s">
         <v>91</v>
       </c>
-      <c r="I22" s="299" t="s">
+      <c r="I22" s="310" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="23" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="305"/>
-      <c r="C23" s="302"/>
+      <c r="B23" s="307"/>
+      <c r="C23" s="308"/>
       <c r="D23" s="139" t="s">
         <v>87</v>
       </c>
@@ -3999,15 +4196,15 @@
       <c r="F23" s="139" t="s">
         <v>98</v>
       </c>
-      <c r="G23" s="302"/>
-      <c r="H23" s="302"/>
-      <c r="I23" s="300"/>
+      <c r="G23" s="308"/>
+      <c r="H23" s="308"/>
+      <c r="I23" s="311"/>
     </row>
     <row r="24" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="306" t="s">
+      <c r="B24" s="303" t="s">
         <v>99</v>
       </c>
-      <c r="C24" s="307"/>
+      <c r="C24" s="304"/>
       <c r="D24" s="150">
         <v>1</v>
       </c>
@@ -4032,28 +4229,28 @@
     </row>
     <row r="26" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="27" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B27" s="303" t="s">
+      <c r="B27" s="305" t="s">
         <v>96</v>
       </c>
-      <c r="C27" s="301"/>
-      <c r="D27" s="298" t="s">
+      <c r="C27" s="306"/>
+      <c r="D27" s="309" t="s">
         <v>86</v>
       </c>
-      <c r="E27" s="298"/>
-      <c r="F27" s="298"/>
-      <c r="G27" s="301" t="s">
+      <c r="E27" s="309"/>
+      <c r="F27" s="309"/>
+      <c r="G27" s="306" t="s">
         <v>90</v>
       </c>
-      <c r="H27" s="301" t="s">
+      <c r="H27" s="306" t="s">
         <v>91</v>
       </c>
-      <c r="I27" s="299" t="s">
+      <c r="I27" s="310" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="28" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="305"/>
-      <c r="C28" s="302"/>
+      <c r="B28" s="307"/>
+      <c r="C28" s="308"/>
       <c r="D28" s="139" t="s">
         <v>87</v>
       </c>
@@ -4063,15 +4260,15 @@
       <c r="F28" s="139" t="s">
         <v>89</v>
       </c>
-      <c r="G28" s="302"/>
-      <c r="H28" s="302"/>
-      <c r="I28" s="300"/>
+      <c r="G28" s="308"/>
+      <c r="H28" s="308"/>
+      <c r="I28" s="311"/>
     </row>
     <row r="29" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="306" t="s">
+      <c r="B29" s="303" t="s">
         <v>100</v>
       </c>
-      <c r="C29" s="307"/>
+      <c r="C29" s="304"/>
       <c r="D29" s="150">
         <v>3</v>
       </c>
@@ -4112,11 +4309,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B27:C28"/>
-    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B9:C10"/>
     <mergeCell ref="G27:G28"/>
     <mergeCell ref="H27:H28"/>
     <mergeCell ref="I27:I28"/>
@@ -4126,12 +4324,11 @@
     <mergeCell ref="G22:G23"/>
     <mergeCell ref="H22:H23"/>
     <mergeCell ref="I22:I23"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B9:C10"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B27:C28"/>
+    <mergeCell ref="D27:F27"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4144,7 +4341,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N4" sqref="N4:S11"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4297,20 +4494,20 @@
       </c>
     </row>
     <row r="9" spans="2:11" s="56" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="306" t="s">
+      <c r="C9" s="303" t="s">
         <v>304</v>
       </c>
-      <c r="D9" s="307"/>
-      <c r="E9" s="307"/>
+      <c r="D9" s="304"/>
+      <c r="E9" s="304"/>
       <c r="F9" s="277">
         <f>SUM(F6:F8)</f>
         <v>138411</v>
       </c>
-      <c r="H9" s="306" t="s">
+      <c r="H9" s="303" t="s">
         <v>304</v>
       </c>
-      <c r="I9" s="307"/>
-      <c r="J9" s="307"/>
+      <c r="I9" s="304"/>
+      <c r="J9" s="304"/>
       <c r="K9" s="277">
         <f>SUM(K6:K8)</f>
         <v>42250</v>
@@ -4409,28 +4606,28 @@
       </c>
     </row>
     <row r="14" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="306" t="s">
+      <c r="C14" s="303" t="s">
         <v>307</v>
       </c>
-      <c r="D14" s="307"/>
-      <c r="E14" s="308">
+      <c r="D14" s="304"/>
+      <c r="E14" s="313">
         <f>F12</f>
         <v>553644</v>
       </c>
-      <c r="F14" s="309"/>
-      <c r="H14" s="306" t="s">
+      <c r="F14" s="314"/>
+      <c r="H14" s="303" t="s">
         <v>307</v>
       </c>
-      <c r="I14" s="307"/>
-      <c r="J14" s="308">
+      <c r="I14" s="304"/>
+      <c r="J14" s="313">
         <f>K12</f>
         <v>169000</v>
       </c>
-      <c r="K14" s="309"/>
+      <c r="K14" s="314"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C15" s="310"/>
-      <c r="D15" s="310"/>
+      <c r="C15" s="315"/>
+      <c r="D15" s="315"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
@@ -4504,11 +4701,11 @@
       </c>
     </row>
     <row r="22" spans="3:8" s="56" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="306" t="s">
+      <c r="C22" s="303" t="s">
         <v>304</v>
       </c>
-      <c r="D22" s="307"/>
-      <c r="E22" s="307"/>
+      <c r="D22" s="304"/>
+      <c r="E22" s="304"/>
       <c r="F22" s="277">
         <f>SUM(F19:F21)</f>
         <v>45292</v>
@@ -4581,15 +4778,15 @@
       <c r="H27" s="56"/>
     </row>
     <row r="28" spans="3:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C28" s="306" t="s">
+      <c r="C28" s="303" t="s">
         <v>307</v>
       </c>
-      <c r="D28" s="307"/>
-      <c r="E28" s="308">
+      <c r="D28" s="304"/>
+      <c r="E28" s="313">
         <f>SUM(F25:F27)</f>
         <v>291168</v>
       </c>
-      <c r="F28" s="309"/>
+      <c r="F28" s="314"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -4803,7 +5000,7 @@
   <dimension ref="B2:K32"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5456,7 +5653,7 @@
   <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6772,8 +6969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8105,7 +8302,7 @@
   <dimension ref="B2:L31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8698,7 +8895,7 @@
       </c>
     </row>
     <row r="4" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="315" t="s">
+      <c r="C4" s="301" t="s">
         <v>299</v>
       </c>
       <c r="D4" s="151">
@@ -8707,7 +8904,7 @@
       <c r="E4" s="151">
         <v>250</v>
       </c>
-      <c r="F4" s="316">
+      <c r="F4" s="302">
         <f>D4*E4</f>
         <v>42250</v>
       </c>
@@ -8732,7 +8929,7 @@
       <c r="C7" s="278" t="s">
         <v>299</v>
       </c>
-      <c r="D7" s="311">
+      <c r="D7" s="299">
         <v>3</v>
       </c>
       <c r="E7" s="142">
@@ -8748,7 +8945,7 @@
       <c r="C8" s="233" t="s">
         <v>353</v>
       </c>
-      <c r="D8" s="312">
+      <c r="D8" s="300">
         <v>2</v>
       </c>
       <c r="E8" s="4">
@@ -8760,15 +8957,15 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="306" t="s">
+      <c r="C9" s="303" t="s">
         <v>354</v>
       </c>
-      <c r="D9" s="307"/>
-      <c r="E9" s="313">
+      <c r="D9" s="304"/>
+      <c r="E9" s="316">
         <f>SUM(F7:F8)</f>
         <v>620000</v>
       </c>
-      <c r="F9" s="314"/>
+      <c r="F9" s="317"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -8778,4 +8975,2064 @@
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:R55"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="23.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5" style="298" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="49.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="9" style="1"/>
+    <col min="12" max="12" width="10.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+    </row>
+    <row r="3" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="318" t="s">
+        <v>357</v>
+      </c>
+      <c r="D3" s="318" t="s">
+        <v>355</v>
+      </c>
+      <c r="E3" s="319" t="s">
+        <v>358</v>
+      </c>
+      <c r="F3" s="159" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="161" t="s">
+        <v>104</v>
+      </c>
+      <c r="L3" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="O3" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="P3" s="32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B4" s="333" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" s="334" t="s">
+        <v>356</v>
+      </c>
+      <c r="D4" s="335"/>
+      <c r="E4" s="335"/>
+      <c r="F4" s="336" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="335">
+        <v>1</v>
+      </c>
+      <c r="H4" s="336" t="s">
+        <v>120</v>
+      </c>
+      <c r="I4" s="358">
+        <v>10</v>
+      </c>
+      <c r="J4" s="358">
+        <v>110</v>
+      </c>
+      <c r="K4" s="359">
+        <v>110</v>
+      </c>
+      <c r="L4" s="358">
+        <v>20</v>
+      </c>
+      <c r="M4" s="360"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="336" t="s">
+        <v>121</v>
+      </c>
+      <c r="P4" s="37"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B5" s="337" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="D5" s="339"/>
+      <c r="E5" s="339"/>
+      <c r="F5" s="340" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="339">
+        <v>1</v>
+      </c>
+      <c r="H5" s="340" t="s">
+        <v>123</v>
+      </c>
+      <c r="I5" s="361">
+        <v>10</v>
+      </c>
+      <c r="J5" s="361">
+        <v>220</v>
+      </c>
+      <c r="K5" s="357">
+        <v>220</v>
+      </c>
+      <c r="L5" s="361">
+        <v>20</v>
+      </c>
+      <c r="M5" s="321"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="340" t="s">
+        <v>124</v>
+      </c>
+      <c r="P5" s="39"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B6" s="337" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="D6" s="339"/>
+      <c r="E6" s="339"/>
+      <c r="F6" s="340" t="s">
+        <v>147</v>
+      </c>
+      <c r="G6" s="339">
+        <v>1</v>
+      </c>
+      <c r="H6" s="340" t="s">
+        <v>148</v>
+      </c>
+      <c r="I6" s="361">
+        <v>10</v>
+      </c>
+      <c r="J6" s="361">
+        <v>20</v>
+      </c>
+      <c r="K6" s="357">
+        <v>40</v>
+      </c>
+      <c r="L6" s="361">
+        <v>20</v>
+      </c>
+      <c r="M6" s="321"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="340" t="s">
+        <v>149</v>
+      </c>
+      <c r="P6" s="39"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B7" s="337" t="s">
+        <v>150</v>
+      </c>
+      <c r="C7" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="D7" s="339"/>
+      <c r="E7" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="F7" s="340" t="s">
+        <v>147</v>
+      </c>
+      <c r="G7" s="339">
+        <v>1</v>
+      </c>
+      <c r="H7" s="340" t="s">
+        <v>151</v>
+      </c>
+      <c r="I7" s="361">
+        <v>10</v>
+      </c>
+      <c r="J7" s="361">
+        <v>20</v>
+      </c>
+      <c r="K7" s="357">
+        <v>20</v>
+      </c>
+      <c r="L7" s="361">
+        <v>40</v>
+      </c>
+      <c r="M7" s="321"/>
+      <c r="N7" s="34"/>
+      <c r="O7" s="340" t="s">
+        <v>152</v>
+      </c>
+      <c r="P7" s="39"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B8" s="337" t="s">
+        <v>157</v>
+      </c>
+      <c r="C8" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="D8" s="339"/>
+      <c r="E8" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="F8" s="340" t="s">
+        <v>147</v>
+      </c>
+      <c r="G8" s="339">
+        <v>1</v>
+      </c>
+      <c r="H8" s="340" t="s">
+        <v>158</v>
+      </c>
+      <c r="I8" s="361">
+        <v>10</v>
+      </c>
+      <c r="J8" s="361">
+        <v>20</v>
+      </c>
+      <c r="K8" s="357">
+        <v>20</v>
+      </c>
+      <c r="L8" s="361">
+        <v>40</v>
+      </c>
+      <c r="M8" s="321"/>
+      <c r="N8" s="34"/>
+      <c r="O8" s="341" t="s">
+        <v>159</v>
+      </c>
+      <c r="P8" s="39"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B9" s="337" t="s">
+        <v>153</v>
+      </c>
+      <c r="C9" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="D9" s="339"/>
+      <c r="E9" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="F9" s="340" t="s">
+        <v>147</v>
+      </c>
+      <c r="G9" s="339">
+        <v>1</v>
+      </c>
+      <c r="H9" s="340" t="s">
+        <v>154</v>
+      </c>
+      <c r="I9" s="361">
+        <v>10</v>
+      </c>
+      <c r="J9" s="361">
+        <v>40</v>
+      </c>
+      <c r="K9" s="357">
+        <v>250</v>
+      </c>
+      <c r="L9" s="361">
+        <v>20</v>
+      </c>
+      <c r="M9" s="321"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="341" t="s">
+        <v>155</v>
+      </c>
+      <c r="P9" s="39"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B10" s="323" t="s">
+        <v>189</v>
+      </c>
+      <c r="C10" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="D10" s="325"/>
+      <c r="E10" s="325"/>
+      <c r="F10" s="58" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" s="325">
+        <v>1</v>
+      </c>
+      <c r="H10" s="58" t="s">
+        <v>190</v>
+      </c>
+      <c r="I10" s="357">
+        <v>10</v>
+      </c>
+      <c r="J10" s="357">
+        <v>140</v>
+      </c>
+      <c r="K10" s="357">
+        <v>140</v>
+      </c>
+      <c r="L10" s="357">
+        <v>10</v>
+      </c>
+      <c r="M10" s="321"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="58" t="s">
+        <v>191</v>
+      </c>
+      <c r="P10" s="39"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B11" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="C11" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34" t="s">
+        <v>287</v>
+      </c>
+      <c r="G11" s="22">
+        <v>1</v>
+      </c>
+      <c r="H11" s="34" t="s">
+        <v>288</v>
+      </c>
+      <c r="I11" s="321">
+        <v>1</v>
+      </c>
+      <c r="J11" s="321">
+        <v>3520</v>
+      </c>
+      <c r="K11" s="321">
+        <f>J11*L11</f>
+        <v>7040</v>
+      </c>
+      <c r="L11" s="321">
+        <v>2</v>
+      </c>
+      <c r="M11" s="321"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="342" t="s">
+        <v>289</v>
+      </c>
+      <c r="P11" s="39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B12" s="337" t="s">
+        <v>142</v>
+      </c>
+      <c r="C12" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="D12" s="339"/>
+      <c r="E12" s="339"/>
+      <c r="F12" s="340" t="s">
+        <v>143</v>
+      </c>
+      <c r="G12" s="339">
+        <v>1</v>
+      </c>
+      <c r="H12" s="340" t="s">
+        <v>144</v>
+      </c>
+      <c r="I12" s="361">
+        <v>1</v>
+      </c>
+      <c r="J12" s="361">
+        <v>720</v>
+      </c>
+      <c r="K12" s="357">
+        <v>1270</v>
+      </c>
+      <c r="L12" s="361">
+        <v>20</v>
+      </c>
+      <c r="M12" s="321"/>
+      <c r="N12" s="34"/>
+      <c r="O12" s="340" t="s">
+        <v>145</v>
+      </c>
+      <c r="P12" s="39"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B13" s="320" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="D13" s="246"/>
+      <c r="E13" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="F13" s="246" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="22">
+        <v>3</v>
+      </c>
+      <c r="H13" s="246" t="s">
+        <v>53</v>
+      </c>
+      <c r="I13" s="321">
+        <v>1</v>
+      </c>
+      <c r="J13" s="321">
+        <v>60</v>
+      </c>
+      <c r="K13" s="321">
+        <f>J13*L13</f>
+        <v>7200</v>
+      </c>
+      <c r="L13" s="321">
+        <v>120</v>
+      </c>
+      <c r="M13" s="321"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="342" t="s">
+        <v>54</v>
+      </c>
+      <c r="P13" s="39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B14" s="337" t="s">
+        <v>160</v>
+      </c>
+      <c r="C14" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="D14" s="339"/>
+      <c r="E14" s="339"/>
+      <c r="F14" s="340" t="s">
+        <v>161</v>
+      </c>
+      <c r="G14" s="339">
+        <v>1</v>
+      </c>
+      <c r="H14" s="340" t="s">
+        <v>162</v>
+      </c>
+      <c r="I14" s="361">
+        <v>50</v>
+      </c>
+      <c r="J14" s="361">
+        <v>160</v>
+      </c>
+      <c r="K14" s="357">
+        <v>160</v>
+      </c>
+      <c r="L14" s="361">
+        <v>50</v>
+      </c>
+      <c r="M14" s="321"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="340" t="s">
+        <v>163</v>
+      </c>
+      <c r="P14" s="39"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B15" s="337" t="s">
+        <v>116</v>
+      </c>
+      <c r="C15" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="D15" s="339"/>
+      <c r="E15" s="339"/>
+      <c r="F15" s="340" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" s="339">
+        <v>1</v>
+      </c>
+      <c r="H15" s="340" t="s">
+        <v>117</v>
+      </c>
+      <c r="I15" s="361">
+        <v>10</v>
+      </c>
+      <c r="J15" s="361">
+        <v>380</v>
+      </c>
+      <c r="K15" s="357">
+        <v>380</v>
+      </c>
+      <c r="L15" s="361">
+        <v>10</v>
+      </c>
+      <c r="M15" s="321"/>
+      <c r="N15" s="34"/>
+      <c r="O15" s="340" t="s">
+        <v>118</v>
+      </c>
+      <c r="P15" s="39"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B16" s="337" t="s">
+        <v>129</v>
+      </c>
+      <c r="C16" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="D16" s="339"/>
+      <c r="E16" s="339"/>
+      <c r="F16" s="340" t="s">
+        <v>130</v>
+      </c>
+      <c r="G16" s="339">
+        <v>1</v>
+      </c>
+      <c r="H16" s="340" t="s">
+        <v>131</v>
+      </c>
+      <c r="I16" s="361">
+        <v>1</v>
+      </c>
+      <c r="J16" s="361">
+        <v>420</v>
+      </c>
+      <c r="K16" s="357">
+        <v>350</v>
+      </c>
+      <c r="L16" s="361">
+        <v>20</v>
+      </c>
+      <c r="M16" s="321"/>
+      <c r="N16" s="34"/>
+      <c r="O16" s="340" t="s">
+        <v>132</v>
+      </c>
+      <c r="P16" s="39"/>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B17" s="337" t="s">
+        <v>125</v>
+      </c>
+      <c r="C17" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="D17" s="339"/>
+      <c r="E17" s="339"/>
+      <c r="F17" s="340" t="s">
+        <v>126</v>
+      </c>
+      <c r="G17" s="339">
+        <v>1</v>
+      </c>
+      <c r="H17" s="340" t="s">
+        <v>127</v>
+      </c>
+      <c r="I17" s="361">
+        <v>1</v>
+      </c>
+      <c r="J17" s="361">
+        <v>260</v>
+      </c>
+      <c r="K17" s="357">
+        <v>320</v>
+      </c>
+      <c r="L17" s="361">
+        <v>20</v>
+      </c>
+      <c r="M17" s="321"/>
+      <c r="N17" s="34"/>
+      <c r="O17" s="340" t="s">
+        <v>128</v>
+      </c>
+      <c r="P17" s="39"/>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B18" s="337" t="s">
+        <v>175</v>
+      </c>
+      <c r="C18" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="D18" s="339"/>
+      <c r="E18" s="339"/>
+      <c r="F18" s="340" t="s">
+        <v>176</v>
+      </c>
+      <c r="G18" s="339">
+        <v>1</v>
+      </c>
+      <c r="H18" s="340" t="s">
+        <v>177</v>
+      </c>
+      <c r="I18" s="361">
+        <v>1</v>
+      </c>
+      <c r="J18" s="361">
+        <v>2850</v>
+      </c>
+      <c r="K18" s="357">
+        <v>3240</v>
+      </c>
+      <c r="L18" s="361">
+        <v>20</v>
+      </c>
+      <c r="M18" s="321"/>
+      <c r="N18" s="34"/>
+      <c r="O18" s="340" t="s">
+        <v>178</v>
+      </c>
+      <c r="P18" s="39"/>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B19" s="337" t="s">
+        <v>179</v>
+      </c>
+      <c r="C19" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="D19" s="339"/>
+      <c r="E19" s="339"/>
+      <c r="F19" s="340" t="s">
+        <v>176</v>
+      </c>
+      <c r="G19" s="339">
+        <v>1</v>
+      </c>
+      <c r="H19" s="340" t="s">
+        <v>180</v>
+      </c>
+      <c r="I19" s="361">
+        <v>1</v>
+      </c>
+      <c r="J19" s="361">
+        <v>1750</v>
+      </c>
+      <c r="K19" s="357">
+        <v>1000</v>
+      </c>
+      <c r="L19" s="361">
+        <v>60</v>
+      </c>
+      <c r="M19" s="321"/>
+      <c r="N19" s="34"/>
+      <c r="O19" s="340" t="s">
+        <v>181</v>
+      </c>
+      <c r="P19" s="39"/>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B20" s="337" t="s">
+        <v>138</v>
+      </c>
+      <c r="C20" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="D20" s="339"/>
+      <c r="E20" s="339"/>
+      <c r="F20" s="340" t="s">
+        <v>139</v>
+      </c>
+      <c r="G20" s="339">
+        <v>1</v>
+      </c>
+      <c r="H20" s="340" t="s">
+        <v>140</v>
+      </c>
+      <c r="I20" s="361">
+        <v>1</v>
+      </c>
+      <c r="J20" s="361">
+        <v>480</v>
+      </c>
+      <c r="K20" s="357">
+        <v>260</v>
+      </c>
+      <c r="L20" s="361">
+        <v>100</v>
+      </c>
+      <c r="M20" s="321"/>
+      <c r="N20" s="34"/>
+      <c r="O20" s="340" t="s">
+        <v>141</v>
+      </c>
+      <c r="P20" s="39"/>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B21" s="337" t="s">
+        <v>171</v>
+      </c>
+      <c r="C21" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="D21" s="339"/>
+      <c r="E21" s="339"/>
+      <c r="F21" s="340" t="s">
+        <v>172</v>
+      </c>
+      <c r="G21" s="339">
+        <v>1</v>
+      </c>
+      <c r="H21" s="340" t="s">
+        <v>173</v>
+      </c>
+      <c r="I21" s="361">
+        <v>1</v>
+      </c>
+      <c r="J21" s="361">
+        <v>750</v>
+      </c>
+      <c r="K21" s="357">
+        <v>550</v>
+      </c>
+      <c r="L21" s="361">
+        <v>25</v>
+      </c>
+      <c r="M21" s="321"/>
+      <c r="N21" s="34"/>
+      <c r="O21" s="340" t="s">
+        <v>174</v>
+      </c>
+      <c r="P21" s="39"/>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B22" s="337" t="s">
+        <v>134</v>
+      </c>
+      <c r="C22" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="D22" s="339"/>
+      <c r="E22" s="339"/>
+      <c r="F22" s="340" t="s">
+        <v>135</v>
+      </c>
+      <c r="G22" s="339">
+        <v>1</v>
+      </c>
+      <c r="H22" s="340" t="s">
+        <v>136</v>
+      </c>
+      <c r="I22" s="361">
+        <v>1</v>
+      </c>
+      <c r="J22" s="361">
+        <v>2150</v>
+      </c>
+      <c r="K22" s="357">
+        <v>1880</v>
+      </c>
+      <c r="L22" s="361">
+        <v>20</v>
+      </c>
+      <c r="M22" s="321"/>
+      <c r="N22" s="34"/>
+      <c r="O22" s="340" t="s">
+        <v>137</v>
+      </c>
+      <c r="P22" s="39"/>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B23" s="337" t="s">
+        <v>165</v>
+      </c>
+      <c r="C23" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="D23" s="339"/>
+      <c r="E23" s="339"/>
+      <c r="F23" s="340" t="s">
+        <v>166</v>
+      </c>
+      <c r="G23" s="339">
+        <v>3</v>
+      </c>
+      <c r="H23" s="340" t="s">
+        <v>162</v>
+      </c>
+      <c r="I23" s="361">
+        <v>1</v>
+      </c>
+      <c r="J23" s="361">
+        <v>280</v>
+      </c>
+      <c r="K23" s="357">
+        <v>270</v>
+      </c>
+      <c r="L23" s="361">
+        <v>60</v>
+      </c>
+      <c r="M23" s="321"/>
+      <c r="N23" s="34"/>
+      <c r="O23" s="340" t="s">
+        <v>167</v>
+      </c>
+      <c r="P23" s="39"/>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B24" s="337" t="s">
+        <v>110</v>
+      </c>
+      <c r="C24" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="D24" s="339"/>
+      <c r="E24" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="F24" s="340" t="s">
+        <v>111</v>
+      </c>
+      <c r="G24" s="339">
+        <v>1</v>
+      </c>
+      <c r="H24" s="340" t="s">
+        <v>112</v>
+      </c>
+      <c r="I24" s="361">
+        <v>10</v>
+      </c>
+      <c r="J24" s="361">
+        <v>200</v>
+      </c>
+      <c r="K24" s="357">
+        <v>200</v>
+      </c>
+      <c r="L24" s="361">
+        <v>20</v>
+      </c>
+      <c r="M24" s="321"/>
+      <c r="N24" s="34"/>
+      <c r="O24" s="340" t="s">
+        <v>113</v>
+      </c>
+      <c r="P24" s="39"/>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B25" s="337" t="s">
+        <v>168</v>
+      </c>
+      <c r="C25" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="D25" s="339"/>
+      <c r="E25" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="F25" s="340" t="s">
+        <v>169</v>
+      </c>
+      <c r="G25" s="339">
+        <v>1</v>
+      </c>
+      <c r="H25" s="340" t="s">
+        <v>170</v>
+      </c>
+      <c r="I25" s="361">
+        <v>1</v>
+      </c>
+      <c r="J25" s="361">
+        <v>3970</v>
+      </c>
+      <c r="K25" s="357">
+        <v>2340</v>
+      </c>
+      <c r="L25" s="361">
+        <v>40</v>
+      </c>
+      <c r="M25" s="321"/>
+      <c r="N25" s="34"/>
+      <c r="O25" s="340" t="s">
+        <v>114</v>
+      </c>
+      <c r="P25" s="39"/>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B26" s="337" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="D26" s="339"/>
+      <c r="E26" s="339"/>
+      <c r="F26" s="340" t="s">
+        <v>107</v>
+      </c>
+      <c r="G26" s="339">
+        <v>1</v>
+      </c>
+      <c r="H26" s="340" t="s">
+        <v>108</v>
+      </c>
+      <c r="I26" s="361">
+        <v>1</v>
+      </c>
+      <c r="J26" s="361">
+        <v>520</v>
+      </c>
+      <c r="K26" s="357">
+        <v>380</v>
+      </c>
+      <c r="L26" s="361">
+        <v>20</v>
+      </c>
+      <c r="M26" s="321"/>
+      <c r="N26" s="34"/>
+      <c r="O26" s="340" t="s">
+        <v>109</v>
+      </c>
+      <c r="P26" s="39"/>
+      <c r="Q26" s="1"/>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B27" s="337" t="s">
+        <v>182</v>
+      </c>
+      <c r="C27" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="D27" s="339"/>
+      <c r="E27" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="F27" s="340" t="s">
+        <v>176</v>
+      </c>
+      <c r="G27" s="339">
+        <v>1</v>
+      </c>
+      <c r="H27" s="340" t="s">
+        <v>183</v>
+      </c>
+      <c r="I27" s="361">
+        <v>5</v>
+      </c>
+      <c r="J27" s="361">
+        <v>870</v>
+      </c>
+      <c r="K27" s="357">
+        <v>870</v>
+      </c>
+      <c r="L27" s="361">
+        <v>40</v>
+      </c>
+      <c r="M27" s="321"/>
+      <c r="N27" s="34"/>
+      <c r="O27" s="340" t="s">
+        <v>184</v>
+      </c>
+      <c r="P27" s="39"/>
+      <c r="Q27" s="1"/>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B28" s="326" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="327"/>
+      <c r="D28" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="E28" s="338"/>
+      <c r="F28" s="338"/>
+      <c r="G28" s="328">
+        <v>1</v>
+      </c>
+      <c r="H28" s="329" t="s">
+        <v>2</v>
+      </c>
+      <c r="I28" s="321">
+        <v>50</v>
+      </c>
+      <c r="J28" s="321">
+        <v>100</v>
+      </c>
+      <c r="K28" s="321"/>
+      <c r="L28" s="321">
+        <v>50</v>
+      </c>
+      <c r="M28" s="321">
+        <f>J28*L28</f>
+        <v>5000</v>
+      </c>
+      <c r="N28" s="34"/>
+      <c r="O28" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="P28" s="39" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B29" s="326" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="327"/>
+      <c r="D29" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="E29" s="338"/>
+      <c r="F29" s="338"/>
+      <c r="G29" s="328">
+        <v>2</v>
+      </c>
+      <c r="H29" s="329" t="s">
+        <v>23</v>
+      </c>
+      <c r="I29" s="321">
+        <v>1</v>
+      </c>
+      <c r="J29" s="321">
+        <v>1260</v>
+      </c>
+      <c r="K29" s="321"/>
+      <c r="L29" s="321">
+        <v>6</v>
+      </c>
+      <c r="M29" s="321">
+        <f>J29*L29</f>
+        <v>7560</v>
+      </c>
+      <c r="N29" s="34"/>
+      <c r="O29" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="P29" s="39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B30" s="343" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="344"/>
+      <c r="D30" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="E30" s="338"/>
+      <c r="F30" s="338"/>
+      <c r="G30" s="22">
+        <v>2</v>
+      </c>
+      <c r="H30" s="345" t="s">
+        <v>352</v>
+      </c>
+      <c r="I30" s="321">
+        <v>1</v>
+      </c>
+      <c r="J30" s="321">
+        <v>960</v>
+      </c>
+      <c r="K30" s="321"/>
+      <c r="L30" s="321">
+        <v>20</v>
+      </c>
+      <c r="M30" s="321">
+        <v>16400</v>
+      </c>
+      <c r="N30" s="34"/>
+      <c r="O30" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="P30" s="322" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B31" s="323" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="324"/>
+      <c r="D31" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="E31" s="338"/>
+      <c r="F31" s="338"/>
+      <c r="G31" s="325">
+        <v>10</v>
+      </c>
+      <c r="H31" s="324" t="s">
+        <v>39</v>
+      </c>
+      <c r="I31" s="321">
+        <v>5</v>
+      </c>
+      <c r="J31" s="321">
+        <v>2280</v>
+      </c>
+      <c r="K31" s="321"/>
+      <c r="L31" s="321">
+        <v>10</v>
+      </c>
+      <c r="M31" s="321">
+        <f>J31*L31</f>
+        <v>22800</v>
+      </c>
+      <c r="N31" s="34"/>
+      <c r="O31" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="P31" s="39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B32" s="326" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="327"/>
+      <c r="D32" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="E32" s="338"/>
+      <c r="F32" s="338"/>
+      <c r="G32" s="328">
+        <v>1</v>
+      </c>
+      <c r="H32" s="329" t="s">
+        <v>24</v>
+      </c>
+      <c r="I32" s="321">
+        <v>2</v>
+      </c>
+      <c r="J32" s="321">
+        <v>7100</v>
+      </c>
+      <c r="K32" s="321"/>
+      <c r="L32" s="321">
+        <v>2</v>
+      </c>
+      <c r="M32" s="321">
+        <f>J32*L32</f>
+        <v>14200</v>
+      </c>
+      <c r="N32" s="34"/>
+      <c r="O32" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="P32" s="39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B33" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="53"/>
+      <c r="D33" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="E33" s="338"/>
+      <c r="F33" s="338"/>
+      <c r="G33" s="22">
+        <v>1</v>
+      </c>
+      <c r="H33" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="I33" s="321">
+        <v>1</v>
+      </c>
+      <c r="J33" s="321">
+        <v>11090</v>
+      </c>
+      <c r="K33" s="321"/>
+      <c r="L33" s="321">
+        <v>2</v>
+      </c>
+      <c r="M33" s="321">
+        <f>J33*L33</f>
+        <v>22180</v>
+      </c>
+      <c r="N33" s="34"/>
+      <c r="O33" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="P33" s="39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B34" s="330" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" s="331"/>
+      <c r="D34" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="E34" s="338"/>
+      <c r="F34" s="338"/>
+      <c r="G34" s="328">
+        <v>1</v>
+      </c>
+      <c r="H34" s="329" t="s">
+        <v>24</v>
+      </c>
+      <c r="I34" s="321">
+        <v>2</v>
+      </c>
+      <c r="J34" s="321">
+        <v>13200</v>
+      </c>
+      <c r="K34" s="321"/>
+      <c r="L34" s="321">
+        <v>4</v>
+      </c>
+      <c r="M34" s="321">
+        <f>J34*L34</f>
+        <v>52800</v>
+      </c>
+      <c r="N34" s="34"/>
+      <c r="O34" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="P34" s="39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B35" s="326" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="327"/>
+      <c r="D35" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="E35" s="338"/>
+      <c r="F35" s="58" t="s">
+        <v>64</v>
+      </c>
+      <c r="G35" s="328">
+        <v>1</v>
+      </c>
+      <c r="H35" s="329" t="s">
+        <v>22</v>
+      </c>
+      <c r="I35" s="321">
+        <v>100</v>
+      </c>
+      <c r="J35" s="321">
+        <v>130</v>
+      </c>
+      <c r="K35" s="321"/>
+      <c r="L35" s="321">
+        <v>100</v>
+      </c>
+      <c r="M35" s="321">
+        <f>J35*L35</f>
+        <v>13000</v>
+      </c>
+      <c r="N35" s="34"/>
+      <c r="O35" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="P35" s="39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B36" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" s="332"/>
+      <c r="D36" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="E36" s="338"/>
+      <c r="F36" s="58" t="s">
+        <v>64</v>
+      </c>
+      <c r="G36" s="328">
+        <v>1</v>
+      </c>
+      <c r="H36" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="I36" s="321">
+        <v>5</v>
+      </c>
+      <c r="J36" s="321">
+        <v>210</v>
+      </c>
+      <c r="K36" s="321"/>
+      <c r="L36" s="321">
+        <v>30</v>
+      </c>
+      <c r="M36" s="321">
+        <f>J36*L36</f>
+        <v>6300</v>
+      </c>
+      <c r="N36" s="34"/>
+      <c r="O36" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="P36" s="39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B37" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="332"/>
+      <c r="D37" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="E37" s="338"/>
+      <c r="F37" s="58" t="s">
+        <v>64</v>
+      </c>
+      <c r="G37" s="328">
+        <v>4</v>
+      </c>
+      <c r="H37" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="I37" s="321">
+        <v>100</v>
+      </c>
+      <c r="J37" s="321">
+        <v>20</v>
+      </c>
+      <c r="K37" s="321"/>
+      <c r="L37" s="356">
+        <v>200</v>
+      </c>
+      <c r="M37" s="321">
+        <f>J37*L37</f>
+        <v>4000</v>
+      </c>
+      <c r="N37" s="346" t="s">
+        <v>41</v>
+      </c>
+      <c r="O37" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="P37" s="39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B38" s="323" t="s">
+        <v>193</v>
+      </c>
+      <c r="C38" s="325"/>
+      <c r="D38" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="E38" s="338"/>
+      <c r="F38" s="58" t="s">
+        <v>64</v>
+      </c>
+      <c r="G38" s="325">
+        <v>1</v>
+      </c>
+      <c r="H38" s="58" t="s">
+        <v>194</v>
+      </c>
+      <c r="I38" s="357">
+        <v>10</v>
+      </c>
+      <c r="J38" s="357">
+        <v>230</v>
+      </c>
+      <c r="K38" s="357">
+        <v>230</v>
+      </c>
+      <c r="L38" s="357">
+        <v>20</v>
+      </c>
+      <c r="M38" s="321"/>
+      <c r="N38" s="34"/>
+      <c r="O38" s="58" t="s">
+        <v>195</v>
+      </c>
+      <c r="P38" s="39"/>
+    </row>
+    <row r="39" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B39" s="323" t="s">
+        <v>196</v>
+      </c>
+      <c r="C39" s="58"/>
+      <c r="D39" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="E39" s="338"/>
+      <c r="F39" s="58" t="s">
+        <v>64</v>
+      </c>
+      <c r="G39" s="325">
+        <v>8</v>
+      </c>
+      <c r="H39" s="58" t="s">
+        <v>198</v>
+      </c>
+      <c r="I39" s="357">
+        <v>300</v>
+      </c>
+      <c r="J39" s="357">
+        <v>130</v>
+      </c>
+      <c r="K39" s="357">
+        <v>130</v>
+      </c>
+      <c r="L39" s="357">
+        <v>300</v>
+      </c>
+      <c r="M39" s="321"/>
+      <c r="N39" s="34"/>
+      <c r="O39" s="58" t="s">
+        <v>197</v>
+      </c>
+      <c r="P39" s="39"/>
+    </row>
+    <row r="40" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B40" s="343" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="344"/>
+      <c r="D40" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="E40" s="338"/>
+      <c r="F40" s="58" t="s">
+        <v>208</v>
+      </c>
+      <c r="G40" s="325">
+        <v>2</v>
+      </c>
+      <c r="H40" s="345" t="s">
+        <v>352</v>
+      </c>
+      <c r="I40" s="357">
+        <v>1</v>
+      </c>
+      <c r="J40" s="357">
+        <v>1020</v>
+      </c>
+      <c r="K40" s="357">
+        <f>J40*L40</f>
+        <v>20400</v>
+      </c>
+      <c r="L40" s="357">
+        <v>20</v>
+      </c>
+      <c r="M40" s="321"/>
+      <c r="N40" s="34"/>
+      <c r="O40" s="58" t="s">
+        <v>293</v>
+      </c>
+      <c r="P40" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q40" s="1"/>
+    </row>
+    <row r="41" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B41" s="323" t="s">
+        <v>209</v>
+      </c>
+      <c r="C41" s="58"/>
+      <c r="D41" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="E41" s="338"/>
+      <c r="F41" s="58" t="s">
+        <v>64</v>
+      </c>
+      <c r="G41" s="325">
+        <v>1</v>
+      </c>
+      <c r="H41" s="58" t="s">
+        <v>210</v>
+      </c>
+      <c r="I41" s="357">
+        <v>100</v>
+      </c>
+      <c r="J41" s="357">
+        <v>130</v>
+      </c>
+      <c r="K41" s="357">
+        <f>J41*L41</f>
+        <v>13000</v>
+      </c>
+      <c r="L41" s="357">
+        <v>100</v>
+      </c>
+      <c r="M41" s="321"/>
+      <c r="N41" s="34"/>
+      <c r="O41" s="347" t="s">
+        <v>294</v>
+      </c>
+      <c r="P41" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q41" s="1"/>
+    </row>
+    <row r="42" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B42" s="320" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" s="348"/>
+      <c r="D42" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="E42" s="338"/>
+      <c r="F42" s="246" t="s">
+        <v>64</v>
+      </c>
+      <c r="G42" s="348">
+        <v>1</v>
+      </c>
+      <c r="H42" s="246" t="s">
+        <v>66</v>
+      </c>
+      <c r="I42" s="362">
+        <v>50</v>
+      </c>
+      <c r="J42" s="362">
+        <v>210</v>
+      </c>
+      <c r="K42" s="362">
+        <v>10500</v>
+      </c>
+      <c r="L42" s="362">
+        <v>50</v>
+      </c>
+      <c r="M42" s="321"/>
+      <c r="N42" s="34"/>
+      <c r="O42" s="342" t="s">
+        <v>67</v>
+      </c>
+      <c r="P42" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q42" s="1"/>
+    </row>
+    <row r="43" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B43" s="320" t="s">
+        <v>68</v>
+      </c>
+      <c r="C43" s="348"/>
+      <c r="D43" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="E43" s="338"/>
+      <c r="F43" s="246" t="s">
+        <v>64</v>
+      </c>
+      <c r="G43" s="348">
+        <v>1</v>
+      </c>
+      <c r="H43" s="246" t="s">
+        <v>69</v>
+      </c>
+      <c r="I43" s="362">
+        <v>10</v>
+      </c>
+      <c r="J43" s="362">
+        <v>210</v>
+      </c>
+      <c r="K43" s="362">
+        <v>2100</v>
+      </c>
+      <c r="L43" s="362">
+        <v>10</v>
+      </c>
+      <c r="M43" s="321"/>
+      <c r="N43" s="34"/>
+      <c r="O43" s="342" t="s">
+        <v>70</v>
+      </c>
+      <c r="P43" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q43" s="1"/>
+    </row>
+    <row r="44" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B44" s="320" t="s">
+        <v>71</v>
+      </c>
+      <c r="C44" s="348"/>
+      <c r="D44" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="E44" s="338"/>
+      <c r="F44" s="246"/>
+      <c r="G44" s="348">
+        <v>2</v>
+      </c>
+      <c r="H44" s="246" t="s">
+        <v>72</v>
+      </c>
+      <c r="I44" s="362">
+        <v>100</v>
+      </c>
+      <c r="J44" s="362">
+        <v>80</v>
+      </c>
+      <c r="K44" s="362">
+        <v>4000</v>
+      </c>
+      <c r="L44" s="362">
+        <v>100</v>
+      </c>
+      <c r="M44" s="321"/>
+      <c r="N44" s="34"/>
+      <c r="O44" s="342" t="s">
+        <v>73</v>
+      </c>
+      <c r="P44" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q44" s="1"/>
+    </row>
+    <row r="45" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B45" s="320" t="s">
+        <v>75</v>
+      </c>
+      <c r="C45" s="246"/>
+      <c r="D45" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="E45" s="338"/>
+      <c r="F45" s="246" t="s">
+        <v>76</v>
+      </c>
+      <c r="G45" s="348">
+        <v>1</v>
+      </c>
+      <c r="H45" s="246" t="s">
+        <v>77</v>
+      </c>
+      <c r="I45" s="362"/>
+      <c r="J45" s="362">
+        <v>270</v>
+      </c>
+      <c r="K45" s="362">
+        <v>0</v>
+      </c>
+      <c r="L45" s="362">
+        <v>20</v>
+      </c>
+      <c r="M45" s="321"/>
+      <c r="N45" s="34"/>
+      <c r="O45" s="246" t="s">
+        <v>78</v>
+      </c>
+      <c r="P45" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q45" s="1"/>
+    </row>
+    <row r="46" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B46" s="320" t="s">
+        <v>79</v>
+      </c>
+      <c r="C46" s="246"/>
+      <c r="D46" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="E46" s="338"/>
+      <c r="F46" s="246" t="s">
+        <v>80</v>
+      </c>
+      <c r="G46" s="348">
+        <v>1</v>
+      </c>
+      <c r="H46" s="246" t="s">
+        <v>79</v>
+      </c>
+      <c r="I46" s="362">
+        <v>10</v>
+      </c>
+      <c r="J46" s="362">
+        <v>200</v>
+      </c>
+      <c r="K46" s="362">
+        <v>2000</v>
+      </c>
+      <c r="L46" s="362">
+        <v>10</v>
+      </c>
+      <c r="M46" s="321"/>
+      <c r="N46" s="34"/>
+      <c r="O46" s="342" t="s">
+        <v>81</v>
+      </c>
+      <c r="P46" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q46" s="1"/>
+    </row>
+    <row r="47" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B47" s="320" t="s">
+        <v>82</v>
+      </c>
+      <c r="C47" s="246"/>
+      <c r="D47" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="E47" s="338"/>
+      <c r="F47" s="246" t="s">
+        <v>80</v>
+      </c>
+      <c r="G47" s="348">
+        <v>1</v>
+      </c>
+      <c r="H47" s="246" t="s">
+        <v>82</v>
+      </c>
+      <c r="I47" s="362">
+        <v>10</v>
+      </c>
+      <c r="J47" s="362">
+        <v>200</v>
+      </c>
+      <c r="K47" s="362">
+        <v>2000</v>
+      </c>
+      <c r="L47" s="362">
+        <v>10</v>
+      </c>
+      <c r="M47" s="321"/>
+      <c r="N47" s="34"/>
+      <c r="O47" s="342" t="s">
+        <v>83</v>
+      </c>
+      <c r="P47" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q47" s="1"/>
+    </row>
+    <row r="48" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B48" s="349" t="s">
+        <v>332</v>
+      </c>
+      <c r="C48" s="350"/>
+      <c r="D48" s="350"/>
+      <c r="E48" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="F48" s="350" t="s">
+        <v>64</v>
+      </c>
+      <c r="G48" s="366">
+        <v>1</v>
+      </c>
+      <c r="H48" s="350" t="s">
+        <v>340</v>
+      </c>
+      <c r="I48" s="363">
+        <v>100</v>
+      </c>
+      <c r="J48" s="363">
+        <v>50</v>
+      </c>
+      <c r="K48" s="321"/>
+      <c r="L48" s="363">
+        <v>100</v>
+      </c>
+      <c r="M48" s="321">
+        <f>J48*L48</f>
+        <v>5000</v>
+      </c>
+      <c r="N48" s="34"/>
+      <c r="O48" s="351" t="s">
+        <v>346</v>
+      </c>
+      <c r="P48" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="R48" s="1"/>
+    </row>
+    <row r="49" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B49" s="349" t="s">
+        <v>338</v>
+      </c>
+      <c r="C49" s="350"/>
+      <c r="D49" s="350"/>
+      <c r="E49" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="F49" s="350" t="s">
+        <v>337</v>
+      </c>
+      <c r="G49" s="366">
+        <v>1</v>
+      </c>
+      <c r="H49" s="350" t="s">
+        <v>344</v>
+      </c>
+      <c r="I49" s="363">
+        <v>1</v>
+      </c>
+      <c r="J49" s="363">
+        <v>430</v>
+      </c>
+      <c r="K49" s="321"/>
+      <c r="L49" s="363">
+        <v>10</v>
+      </c>
+      <c r="M49" s="321">
+        <f>J49*L49</f>
+        <v>4300</v>
+      </c>
+      <c r="N49" s="34"/>
+      <c r="O49" s="351" t="s">
+        <v>350</v>
+      </c>
+      <c r="P49" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="R49" s="1"/>
+    </row>
+    <row r="50" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B50" s="349" t="s">
+        <v>336</v>
+      </c>
+      <c r="C50" s="350"/>
+      <c r="D50" s="350"/>
+      <c r="E50" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="F50" s="350" t="s">
+        <v>337</v>
+      </c>
+      <c r="G50" s="366">
+        <v>1</v>
+      </c>
+      <c r="H50" s="350" t="s">
+        <v>343</v>
+      </c>
+      <c r="I50" s="363">
+        <v>1</v>
+      </c>
+      <c r="J50" s="363">
+        <v>430</v>
+      </c>
+      <c r="K50" s="321"/>
+      <c r="L50" s="363">
+        <v>10</v>
+      </c>
+      <c r="M50" s="321">
+        <f>J50*L50</f>
+        <v>4300</v>
+      </c>
+      <c r="N50" s="34"/>
+      <c r="O50" s="351" t="s">
+        <v>349</v>
+      </c>
+      <c r="P50" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="R50" s="1"/>
+    </row>
+    <row r="51" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B51" s="349" t="s">
+        <v>333</v>
+      </c>
+      <c r="C51" s="350"/>
+      <c r="D51" s="350"/>
+      <c r="E51" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="F51" s="350" t="s">
+        <v>331</v>
+      </c>
+      <c r="G51" s="366">
+        <v>2</v>
+      </c>
+      <c r="H51" s="350" t="s">
+        <v>341</v>
+      </c>
+      <c r="I51" s="363">
+        <v>1</v>
+      </c>
+      <c r="J51" s="363">
+        <v>290</v>
+      </c>
+      <c r="K51" s="321"/>
+      <c r="L51" s="363">
+        <v>20</v>
+      </c>
+      <c r="M51" s="321">
+        <f>J51*L51</f>
+        <v>5800</v>
+      </c>
+      <c r="N51" s="34"/>
+      <c r="O51" s="351" t="s">
+        <v>347</v>
+      </c>
+      <c r="P51" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="R51" s="1"/>
+    </row>
+    <row r="52" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B52" s="349" t="s">
+        <v>330</v>
+      </c>
+      <c r="C52" s="350"/>
+      <c r="D52" s="350"/>
+      <c r="E52" s="338" t="s">
+        <v>356</v>
+      </c>
+      <c r="F52" s="350" t="s">
+        <v>331</v>
+      </c>
+      <c r="G52" s="366">
+        <v>1</v>
+      </c>
+      <c r="H52" s="350" t="s">
+        <v>339</v>
+      </c>
+      <c r="I52" s="363">
+        <v>1</v>
+      </c>
+      <c r="J52" s="363">
+        <v>30</v>
+      </c>
+      <c r="K52" s="321"/>
+      <c r="L52" s="363">
+        <v>10</v>
+      </c>
+      <c r="M52" s="321">
+        <f>J52*L52</f>
+        <v>300</v>
+      </c>
+      <c r="N52" s="34"/>
+      <c r="O52" s="351" t="s">
+        <v>345</v>
+      </c>
+      <c r="P52" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="R52" s="1"/>
+    </row>
+    <row r="53" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B53" s="352" t="s">
+        <v>334</v>
+      </c>
+      <c r="C53" s="353"/>
+      <c r="D53" s="353"/>
+      <c r="E53" s="354" t="s">
+        <v>356</v>
+      </c>
+      <c r="F53" s="353" t="s">
+        <v>335</v>
+      </c>
+      <c r="G53" s="367">
+        <v>1</v>
+      </c>
+      <c r="H53" s="353" t="s">
+        <v>342</v>
+      </c>
+      <c r="I53" s="364">
+        <v>10</v>
+      </c>
+      <c r="J53" s="364">
+        <v>100</v>
+      </c>
+      <c r="K53" s="365"/>
+      <c r="L53" s="364">
+        <v>10</v>
+      </c>
+      <c r="M53" s="365">
+        <f>J53*L53</f>
+        <v>1000</v>
+      </c>
+      <c r="N53" s="36"/>
+      <c r="O53" s="355" t="s">
+        <v>348</v>
+      </c>
+      <c r="P53" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="R53" s="1"/>
+    </row>
+    <row r="54" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B54" s="55"/>
+      <c r="C54" s="55"/>
+      <c r="D54" s="55"/>
+      <c r="E54" s="55"/>
+      <c r="F54" s="55"/>
+      <c r="G54" s="368"/>
+      <c r="H54" s="55"/>
+      <c r="I54" s="55"/>
+      <c r="J54" s="55"/>
+      <c r="K54" s="55"/>
+      <c r="L54" s="55"/>
+      <c r="M54" s="55"/>
+      <c r="N54" s="55"/>
+      <c r="O54" s="55"/>
+      <c r="P54" s="55"/>
+    </row>
+    <row r="55" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B55" s="55"/>
+      <c r="C55" s="55"/>
+      <c r="D55" s="55"/>
+      <c r="E55" s="55"/>
+      <c r="F55" s="55"/>
+      <c r="G55" s="368"/>
+      <c r="H55" s="55"/>
+      <c r="I55" s="55"/>
+      <c r="J55" s="55"/>
+      <c r="K55" s="55"/>
+      <c r="L55" s="55"/>
+      <c r="M55" s="55"/>
+      <c r="N55" s="55"/>
+      <c r="O55" s="55"/>
+      <c r="P55" s="55"/>
+    </row>
+  </sheetData>
+  <sortState ref="B48:W53">
+    <sortCondition ref="B48:B53"/>
+  </sortState>
+  <phoneticPr fontId="10" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[Pipette] V1.0 Gerber 재송부 - bottom error 수정
</commit_message>
<xml_diff>
--- a/Femto Project 비용 List.xlsx
+++ b/Femto Project 비용 List.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3735" yWindow="1890" windowWidth="28800" windowHeight="12060" activeTab="8"/>
+    <workbookView xWindow="3735" yWindow="1890" windowWidth="28800" windowHeight="12060"/>
   </bookViews>
   <sheets>
     <sheet name="전체 비용 List" sheetId="9" r:id="rId1"/>
@@ -21,12 +21,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4">'0314'!$B$4:$F$4</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="393">
   <si>
     <t>Vendor</t>
   </si>
@@ -50,22 +50,22 @@
   </si>
   <si>
     <t>재고</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>상품코드</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>ICbanQ</t>
   </si>
   <si>
     <t>ICbanQ</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">P002101847 </t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>NTD5802N</t>
@@ -75,11 +75,11 @@
   </si>
   <si>
     <t>53398-0471</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>50058-8000</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>CRIMP TERMINAL 51021용 (1.25mm) AWG 28,30,32</t>
@@ -92,11 +92,11 @@
   </si>
   <si>
     <t>51021-0400</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>구매수량</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>1.25mm 4-Pin Housing, Female</t>
@@ -112,90 +112,90 @@
   </si>
   <si>
     <t>Total</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>P000740132</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>P005634281</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>CTX210609-R</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>TRANSFORMER CCFL 6W 13V 11MA SMD Turn-R:100</t>
   </si>
   <si>
     <t>CTX210605-R</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>P002058985</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>P005831162</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>P002058197</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">P007073878 </t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>부가세</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>부품 Total</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>P007567011</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>NVMFS5C450NL</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>CAP TANT 220UF 16V 10% 2917</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>P008221708</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>장보고 재고 있음</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>2/5일 구매</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>T491D227K016AT</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>재고 없음</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">P007223445 </t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>2/8일 구매</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -223,19 +223,19 @@
       </rPr>
       <t>-R</t>
     </r>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>B180212004001</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>주문번호</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>2/12일 구매</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>BZT52C5V1S</t>
@@ -338,67 +338,67 @@
   </si>
   <si>
     <t>Pipette Main</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>작업기간</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Month</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Day[20/Month]</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Hour[3/Day]</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>시급</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>가중치</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>LF Gen MCU</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>LF Control MCU</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Cost</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>1차 작업</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Item</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>2차 작업</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Hour[3.5/Day]</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>H/W</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>M/E</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Set 수량</t>
@@ -408,11 +408,11 @@
   </si>
   <si>
     <t>구매 Cost</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>ICBanQ 3/14</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>STPS120M</t>
@@ -425,7 +425,7 @@
   </si>
   <si>
     <t>P001539333</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>SMBJ12CA</t>
@@ -438,15 +438,15 @@
   </si>
   <si>
     <t>P004928252</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>P007475431</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>LF용 포함 구매</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>DC-011C_SMD</t>
@@ -456,7 +456,7 @@
   </si>
   <si>
     <t>P005658771</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>053048-0310</t>
@@ -466,7 +466,7 @@
   </si>
   <si>
     <t>P005634294</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>053048-0710</t>
@@ -476,7 +476,7 @@
   </si>
   <si>
     <t>P005634298</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>HI05-AG0272</t>
@@ -489,7 +489,7 @@
   </si>
   <si>
     <t>P005659337</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>F0603E2R50FSTR</t>
@@ -502,11 +502,11 @@
   </si>
   <si>
     <t>P001574681</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>1 point 삭제 예정</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>MSS5131-153ML</t>
@@ -519,7 +519,7 @@
   </si>
   <si>
     <t xml:space="preserve">P002266417 </t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>LQM2HPZ2R2MG0</t>
@@ -532,7 +532,7 @@
   </si>
   <si>
     <t>P008172717</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>ASMT-YTD2-0BB02</t>
@@ -545,7 +545,7 @@
   </si>
   <si>
     <t>P000725384</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>17-21/W1D-ANPHY/3T</t>
@@ -558,7 +558,7 @@
   </si>
   <si>
     <t>P005609815</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>19-21/R6C-AP1Q2/3T</t>
@@ -568,7 +568,7 @@
   </si>
   <si>
     <t>P005609821</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>19-217/W1D-APQHY/3T</t>
@@ -578,11 +578,11 @@
   </si>
   <si>
     <t>P000098995</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>재품이 없어 고휘도 구매</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>19-213/G6C-AN1P2 /3T</t>
@@ -592,7 +592,7 @@
   </si>
   <si>
     <t>P005609818</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>CTT-1139P1</t>
@@ -605,11 +605,11 @@
   </si>
   <si>
     <t>P000092681</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>MOQ</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>SKRMABE010</t>
@@ -619,7 +619,7 @@
   </si>
   <si>
     <t xml:space="preserve">P001566090 </t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>STM32F070RBT6</t>
@@ -641,7 +641,7 @@
   </si>
   <si>
     <t>P000166190</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>LM2735XMF</t>
@@ -654,7 +654,7 @@
   </si>
   <si>
     <t>P006290287</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>LM3671MF-3.3</t>
@@ -664,7 +664,7 @@
   </si>
   <si>
     <t>P007302353</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>TPS3801L30</t>
@@ -674,79 +674,79 @@
   </si>
   <si>
     <t>P007092561</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>Pipette Main</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Battery 하네스</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>구매 Cost</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>ICBanQ 3/14</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>51021-0300</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>1.25mm Pitch Housing, Female, 3-Pin</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>P005634252</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>Transformer 하네스</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>51021-0700</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>1.25mm Pitch Housing, Female, 7-Pin</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>P005634256</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>50058 양단 1007 케이블</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>P005634320</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>50058 양단 케이블 L=100mm, Black</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>Date</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Item</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Comment</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Pipette과 overlap되는 LF MCU 부품 구매</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>ON Semiconductor</t>
@@ -759,478 +759,478 @@
   </si>
   <si>
     <t>구매수량</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Total</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>재고</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>주문번호</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>EX-936ESD</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve"> EXSO </t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>정전기 방지 온도조절형 인두, 소비전력:60W, 온도:220℃ ~ 480℃</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>P001909039</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">LedSol 3001 </t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>EXSO</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>디지털 무연인두기, 75W, 온도: 100~500℃</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>P007193509</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">LedSol-100 </t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>아날로그 무연인두기 , 24V 75W, 온도: 200~480℃</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>P007193511</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">LedSol-200 </t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>디지털 무연인두기, 24V 70W, 온도: 200~480℃</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>P007193512</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>FX-888D(70W)</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>HAKKO</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>디지털 무연인두기, 26V 70W, 온도: 200~480℃</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>P005688453</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>FX-951</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>디지털 무연인두기, 24V 75W, 온도: 200~450℃</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>P005688454</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>T18-K</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>HAKKO</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>HAKKO FX-888(FX-8801) 전용 인두 칼팁</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>P002116124</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>T18-3.5K</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>T18-B</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>HAKKO FX-888(FX-8801) 전용 인두 팁</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">P002116123 </t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>B3474</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Rubber Cleaner</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>A1561</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>HAKKO A1561 클리닝와이어</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>P004702618</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>A1559</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>HAKKO A1559 스폰지</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>P004704819</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>SPPON 18</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>HAKKO 18 SPPON DESOLDERING TOOL</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>P004702809</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>18N.18G</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>HAKKO SPPON NOZZLE</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>ic114</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>UL1007-AWG20</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>UL전선</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>극세선 난연성 전선(UL전선) / AWG20 / 길이(30M) (검정색)</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">P002329495 </t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>극세선 난연성 전선(UL전선) / AWG20 / 길이(30M) (빨강)</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">P002329190 </t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>칩저항 키트</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Any vender</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>1005 사이즈 F급(1%) 160종 칩저항 키트 - (100개들이)</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>P001907055</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>JL-0232 적색</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Any vender</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">더블 바나나플러그 / 적색 </t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>P005658758</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>GHG630DCE</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve"> BOSCH </t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>열풍기(히터건) (GHG630DCE)</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>P007320842</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>ST-LINK/V2</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>STMicroelectronics</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>ICD/PROGRAMMER, FOR STM8, STM32</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>P001648331</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>ENGINEER SL-04</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>ENGINEER SL-04 DESK-TOP LOUPE, 렌즈 직경 75mm, 배율 3X</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">P004704041 </t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>8611L</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>8611L LED조명 확대경, 렌즈 직경 89mm, 배율 3X</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>P004704064</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>824-22-003-00-005000</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Mill-Max</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">Mill-Max Pin &amp; Socket Connectors </t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>P008110102</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Transformer PCB</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>재고</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>ICBanQ 3/14</t>
   </si>
   <si>
     <t>P007567011</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>P005634282</t>
-    <phoneticPr fontId="34" type="noConversion"/>
+    <phoneticPr fontId="35" type="noConversion"/>
   </si>
   <si>
     <t>재고 소진</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Pipette V1.0 부품 및 장비</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>실험실에서 사용할 장비 및 Pipette 관련 추가 부품</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>부자재</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>수삽</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>개인</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Point</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>단가</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>금액</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>소계</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>작업내용</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>수량</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>합계</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>-</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>-</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>이윤</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>SMD</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Metal mask</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Sample용 견적</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>부품비</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>LF Generator MCU Board</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">HIPPO 6구 접지 멀티탭 멀티탭 - 기본 1.5M </t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">HIPPO 6구 접지 멀티탭 멀티탭 - 3M </t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>HIPPO</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>KFT HT-5023 스트리퍼 (AWG20~30)</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">KFT </t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>P001415029</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>페이스트 [135-0805]</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>P008012287</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>정전기매트 120cm*1M</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>P000119604</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">P007311227 </t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>실험실 물품 구매</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>제이엘텍 - Sample build 견적</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>LF GEN MCU 부품 구매</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>HEADER_2.54mm_2x5</t>
@@ -1297,71 +1297,71 @@
   </si>
   <si>
     <t>Exso</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>40V, 2.8mOhm , 110A, Single N−Channel Power MOSFET</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>PCB Artwork</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Total</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Transformer</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>O</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Pipette Main</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>LF MCU</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>LF GEN MCU Layout 및 제작비</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>구매비용</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Pipette Proto-type 부품 구매</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Transformer V1.0 부품 구매</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>계약금액</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Touch Program</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Pipette</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Proto-type</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>V1.0</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Touch PC - New</t>
@@ -1374,115 +1374,119 @@
   </si>
   <si>
     <t>S/W 개발비</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Date</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Model</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Pipette</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Proto</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Version</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>수량</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>단가</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>작업 내용</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Layout</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>금액</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>제작</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>PCB</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Main</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Transformer</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>V1.0</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>LF</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Gen MCU</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pipette Transformer Layout 및 제작비</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pipette Proto-type Layout 및 제작비</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>H/W Layout 및 Manual Solder 비용</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pipette Proto-type F/W 개발비</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>H/W 개발비</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>S/W 개발비</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>P004707690</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>NA645</t>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
     <t>Pipette V1.0 / LF MCU 일부</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pipette Transformer Layout 및 제작비</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pipette Proto-type Layout 및 제작비</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>H/W Layout 및 Manual Solder 비용</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pipette Proto-type F/W 개발비</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>Total</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>H/W 개발비</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>S/W 개발비</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>P004707690</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>NA645</t>
-    <phoneticPr fontId="11" type="noConversion"/>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pipette Main V1.0 PCB 제작</t>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1500,12 +1504,20 @@
     <numFmt numFmtId="181" formatCode="0.0\ &quot;ea&quot;"/>
     <numFmt numFmtId="182" formatCode="0.0\ &quot;일&quot;"/>
   </numFmts>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2567,283 +2579,283 @@
   </borders>
   <cellStyleXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="41" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2862,7 +2874,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="43" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="43" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2871,7 +2883,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="43" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="43" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2886,32 +2898,32 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="29" fillId="33" borderId="11" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="30" fillId="33" borderId="11" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="43" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="29" fillId="33" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="43" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="30" fillId="33" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="43" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="43" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="43" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="43" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="43" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="43" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="43" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="43" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="52" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="52" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2925,21 +2937,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="52" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="52" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="52" applyFill="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="41" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="41" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="176" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2952,26 +2964,26 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="29" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="30" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="16" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="36" borderId="16" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="17" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="36" borderId="17" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="17" xfId="43" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="11" fillId="36" borderId="17" xfId="43" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2984,13 +2996,13 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="43" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="43" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -3003,16 +3015,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="30" fillId="34" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="41" fontId="31" fillId="34" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="41" fontId="0" fillId="34" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="41" fontId="0" fillId="34" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -3059,34 +3071,34 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="41" fontId="0" fillId="34" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="41" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="29" fillId="33" borderId="24" xfId="69" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="30" fillId="33" borderId="24" xfId="69" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="35" borderId="25" xfId="69" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="35" borderId="25" xfId="69" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="69" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="29" fillId="33" borderId="11" xfId="69" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="69" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="30" fillId="33" borderId="11" xfId="69" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="35" borderId="12" xfId="69" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="35" borderId="12" xfId="69" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="69" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="69" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="69" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="69" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="69" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="69" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
@@ -3108,60 +3120,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="75" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="75" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="75" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="75" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="75">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="75" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="75">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="75" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="75" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="29" fillId="33" borderId="23" xfId="75" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="30" fillId="0" borderId="0" xfId="75" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="30" fillId="33" borderId="23" xfId="75" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="29" fillId="33" borderId="24" xfId="75" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="30" fillId="33" borderId="24" xfId="75" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="29" fillId="33" borderId="33" xfId="75" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="30" fillId="33" borderId="33" xfId="75" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="29" fillId="33" borderId="23" xfId="69" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="30" fillId="33" borderId="23" xfId="69" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="75" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="75" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="75" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="75" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="75" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="75" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="27" xfId="76" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="75" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="75" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="75" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="75" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="75" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="75" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="26" xfId="76" applyFont="1" applyBorder="1">
@@ -3173,46 +3185,46 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="14" xfId="76" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="15" xfId="75" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="15" xfId="75" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="16" xfId="76" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="69" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="69" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="17" xfId="76" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="18" xfId="75" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="17" xfId="75" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="17" xfId="75" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="18" xfId="75" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="17" xfId="75" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="17" xfId="75" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="26" xfId="76" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="18" xfId="69" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="29" fillId="0" borderId="22" xfId="76" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" xfId="75" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="75" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="18" xfId="69" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="30" fillId="0" borderId="22" xfId="76" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" xfId="75" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" xfId="75" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3221,7 +3233,7 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="29" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="30" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3267,20 +3279,20 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="41" fontId="29" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="41" fontId="30" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="29" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="30" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="29" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="30" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -3296,125 +3308,125 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="29" fillId="33" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="30" fillId="33" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="29" fillId="33" borderId="23" xfId="77" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="30" fillId="33" borderId="23" xfId="77" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="29" fillId="33" borderId="24" xfId="77" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="30" fillId="33" borderId="24" xfId="77" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="77" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="77" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="77" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="77" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="77" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="77" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="37" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="29" fillId="33" borderId="10" xfId="78" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="30" fillId="33" borderId="10" xfId="78" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="29" fillId="33" borderId="11" xfId="78" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="30" fillId="33" borderId="11" xfId="78" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="78" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="78" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="78">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="78" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="78" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="78">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="37" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="78" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="34" borderId="25" xfId="69" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="78" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="34" borderId="25" xfId="69" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="78" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="78" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" xfId="78" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="29" fillId="33" borderId="24" xfId="78" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" xfId="78" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="30" fillId="33" borderId="24" xfId="78" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="78" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="78" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="78" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="14" xfId="79" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="78" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="78" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="14" xfId="79" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="78" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="78" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="78" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="17" xfId="79" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="78" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="78" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="78" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="17" xfId="79" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="78" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="78" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="78" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="20" xfId="79" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="20" xfId="79" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="78" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="78" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" xfId="79" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="78" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="14" xfId="79" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="15" xfId="78" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="78" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="17" xfId="79" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="78" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="78" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="78" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="20" xfId="79" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="20" xfId="79" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="78" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="78" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" xfId="79" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="78" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="14" xfId="79" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="15" xfId="78" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="78" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="17" xfId="79" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="78" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -3427,71 +3439,71 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="29" fillId="33" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="30" fillId="33" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="29" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="41" fontId="30" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="80" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="17" xfId="80" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="80" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="17" xfId="80" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="80" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="80" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="80" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="17" xfId="95" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="34" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="34" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="34" borderId="15" xfId="78" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="34" borderId="18" xfId="80" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="34" borderId="21" xfId="78" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="34" borderId="18" xfId="78" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="34" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="34" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="43" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="80" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="17" xfId="80" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="80" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="17" xfId="80" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="80" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="80" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="80" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="17" xfId="95" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="34" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="34" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="34" borderId="15" xfId="78" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="34" borderId="18" xfId="80" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="34" borderId="21" xfId="78" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="34" borderId="18" xfId="78" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="34" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="34" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="43" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3499,15 +3511,15 @@
     </xf>
     <xf numFmtId="181" fontId="0" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="182" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="29" fillId="33" borderId="34" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="30" fillId="33" borderId="34" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="29" fillId="33" borderId="35" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="30" fillId="33" borderId="35" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="78" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="78" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3525,103 +3537,103 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="43" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="43" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="52" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="75" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="75" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="75" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="75" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="75" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="75" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="75" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="75" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="75" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="75" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="75" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="69" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="17" xfId="78" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="75" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="69" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="17" xfId="78" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="43" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="43" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="78" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="78" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="80" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="80" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="17" xfId="80" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="80" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="80" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="80" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="80" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="17" xfId="80" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="80" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="80" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="20" xfId="80" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="30" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="20" xfId="80" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="31" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3630,25 +3642,25 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="41" fontId="6" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="5" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -3657,23 +3669,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="41" fontId="29" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="30" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="36" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -3685,157 +3697,157 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="36" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="36" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="36" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="36" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="36" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="29" fillId="36" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="30" fillId="36" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="29" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="30" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="29" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="30" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="30" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="31" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="30" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="30" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="31" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="31" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="30" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="31" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="30" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="30" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="31" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="31" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="29" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="30" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="29" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="30" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="29" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="30" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="29" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="30" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="41" fontId="29" fillId="33" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="30" fillId="33" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="29" fillId="33" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="30" fillId="33" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="41" fontId="30" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="31" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="78" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="78" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="30" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="29" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="30" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="41" fontId="29" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="30" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="41" fontId="29" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="29" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="30" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="78" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="78" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="96">
@@ -3942,6 +3954,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -3989,7 +4004,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4024,7 +4039,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4235,8 +4250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:G30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4264,10 +4279,10 @@
         <v>353</v>
       </c>
       <c r="E4" s="384" t="s">
+        <v>387</v>
+      </c>
+      <c r="F4" s="384" t="s">
         <v>388</v>
-      </c>
-      <c r="F4" s="384" t="s">
-        <v>389</v>
       </c>
       <c r="G4" s="385" t="s">
         <v>199</v>
@@ -4275,12 +4290,12 @@
     </row>
     <row r="5" spans="2:7" s="197" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="199" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C5" s="200"/>
       <c r="D5" s="343">
         <f>SUM(D6:D25)</f>
-        <v>1570330</v>
+        <v>1658330</v>
       </c>
       <c r="E5" s="343">
         <f>SUM(E6:E25)</f>
@@ -4297,7 +4312,7 @@
         <v>43062</v>
       </c>
       <c r="C6" s="374" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D6" s="375"/>
       <c r="E6" s="375">
@@ -4311,7 +4326,7 @@
         <v>43062</v>
       </c>
       <c r="C7" s="378" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D7" s="379"/>
       <c r="E7" s="379"/>
@@ -4367,7 +4382,7 @@
         <v>43143</v>
       </c>
       <c r="C11" s="204" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D11" s="349"/>
       <c r="E11" s="349">
@@ -4381,7 +4396,7 @@
         <v>43173</v>
       </c>
       <c r="C12" s="204" t="s">
-        <v>382</v>
+        <v>391</v>
       </c>
       <c r="D12" s="349">
         <v>514080</v>
@@ -4423,9 +4438,15 @@
       <c r="G14" s="371"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="203"/>
-      <c r="C15" s="204"/>
-      <c r="D15" s="349"/>
+      <c r="B15" s="203">
+        <v>43220</v>
+      </c>
+      <c r="C15" s="204" t="s">
+        <v>392</v>
+      </c>
+      <c r="D15" s="349">
+        <v>88000</v>
+      </c>
       <c r="E15" s="349"/>
       <c r="F15" s="389"/>
       <c r="G15" s="371"/>
@@ -4514,7 +4535,7 @@
       <c r="B30" s="194"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
@@ -4735,29 +4756,29 @@
       </c>
     </row>
     <row r="9" spans="2:16" s="56" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="395" t="s">
+      <c r="C9" s="397" t="s">
         <v>297</v>
       </c>
-      <c r="D9" s="396"/>
-      <c r="E9" s="396"/>
+      <c r="D9" s="398"/>
+      <c r="E9" s="398"/>
       <c r="F9" s="265">
         <f>SUM(F6:F8)</f>
         <v>138411</v>
       </c>
-      <c r="H9" s="395" t="s">
+      <c r="H9" s="397" t="s">
         <v>297</v>
       </c>
-      <c r="I9" s="396"/>
-      <c r="J9" s="396"/>
+      <c r="I9" s="398"/>
+      <c r="J9" s="398"/>
       <c r="K9" s="265">
         <f>SUM(K6:K8)</f>
         <v>42250</v>
       </c>
-      <c r="M9" s="395" t="s">
+      <c r="M9" s="397" t="s">
         <v>297</v>
       </c>
-      <c r="N9" s="396"/>
-      <c r="O9" s="396"/>
+      <c r="N9" s="398"/>
+      <c r="O9" s="398"/>
       <c r="P9" s="265">
         <f>SUM(P6:P8)</f>
         <v>44750</v>
@@ -4898,37 +4919,37 @@
       </c>
     </row>
     <row r="14" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="395" t="s">
+      <c r="C14" s="397" t="s">
         <v>300</v>
       </c>
-      <c r="D14" s="396"/>
-      <c r="E14" s="416">
+      <c r="D14" s="398"/>
+      <c r="E14" s="418">
         <f>F12</f>
         <v>553644</v>
       </c>
-      <c r="F14" s="417"/>
-      <c r="H14" s="395" t="s">
+      <c r="F14" s="419"/>
+      <c r="H14" s="397" t="s">
         <v>300</v>
       </c>
-      <c r="I14" s="396"/>
-      <c r="J14" s="416">
+      <c r="I14" s="398"/>
+      <c r="J14" s="418">
         <f>K12</f>
         <v>169000</v>
       </c>
-      <c r="K14" s="417"/>
-      <c r="M14" s="395" t="s">
+      <c r="K14" s="419"/>
+      <c r="M14" s="397" t="s">
         <v>300</v>
       </c>
-      <c r="N14" s="396"/>
-      <c r="O14" s="416">
+      <c r="N14" s="398"/>
+      <c r="O14" s="418">
         <f>P12</f>
         <v>150000</v>
       </c>
-      <c r="P14" s="417"/>
+      <c r="P14" s="419"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="C15" s="418"/>
-      <c r="D15" s="418"/>
+      <c r="C15" s="420"/>
+      <c r="D15" s="420"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
@@ -5002,11 +5023,11 @@
       </c>
     </row>
     <row r="22" spans="3:8" s="56" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="395" t="s">
+      <c r="C22" s="397" t="s">
         <v>297</v>
       </c>
-      <c r="D22" s="396"/>
-      <c r="E22" s="396"/>
+      <c r="D22" s="398"/>
+      <c r="E22" s="398"/>
       <c r="F22" s="265">
         <f>SUM(F19:F21)</f>
         <v>45292</v>
@@ -5079,18 +5100,23 @@
       <c r="H27" s="56"/>
     </row>
     <row r="28" spans="3:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C28" s="395" t="s">
+      <c r="C28" s="397" t="s">
         <v>300</v>
       </c>
-      <c r="D28" s="396"/>
-      <c r="E28" s="416">
+      <c r="D28" s="398"/>
+      <c r="E28" s="418">
         <f>SUM(F25:F27)</f>
         <v>291168</v>
       </c>
-      <c r="F28" s="417"/>
+      <c r="F28" s="419"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="C22:E22"/>
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="E28:F28"/>
     <mergeCell ref="H9:J9"/>
@@ -5099,13 +5125,8 @@
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C15:D15"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="C22:E22"/>
   </mergeCells>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -5138,7 +5159,7 @@
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B2" s="56" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="3" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -5167,22 +5188,22 @@
       <c r="I4" s="262" t="s">
         <v>374</v>
       </c>
-      <c r="K4" s="397" t="s">
+      <c r="K4" s="399" t="s">
         <v>95</v>
       </c>
-      <c r="L4" s="391"/>
-      <c r="M4" s="399" t="s">
+      <c r="L4" s="393"/>
+      <c r="M4" s="401" t="s">
         <v>85</v>
       </c>
-      <c r="N4" s="399"/>
-      <c r="O4" s="399"/>
-      <c r="P4" s="391" t="s">
+      <c r="N4" s="401"/>
+      <c r="O4" s="401"/>
+      <c r="P4" s="393" t="s">
         <v>89</v>
       </c>
-      <c r="Q4" s="391" t="s">
+      <c r="Q4" s="393" t="s">
         <v>90</v>
       </c>
-      <c r="R4" s="393" t="s">
+      <c r="R4" s="395" t="s">
         <v>93</v>
       </c>
     </row>
@@ -5212,8 +5233,8 @@
         <f t="shared" ref="I5:I10" si="0">G5*H5</f>
         <v>750000</v>
       </c>
-      <c r="K5" s="398"/>
-      <c r="L5" s="392"/>
+      <c r="K5" s="400"/>
+      <c r="L5" s="394"/>
       <c r="M5" s="387" t="s">
         <v>86</v>
       </c>
@@ -5223,9 +5244,9 @@
       <c r="O5" s="387" t="s">
         <v>97</v>
       </c>
-      <c r="P5" s="392"/>
-      <c r="Q5" s="392"/>
-      <c r="R5" s="394"/>
+      <c r="P5" s="394"/>
+      <c r="Q5" s="394"/>
+      <c r="R5" s="396"/>
     </row>
     <row r="6" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="203">
@@ -5253,10 +5274,10 @@
         <f t="shared" si="0"/>
         <v>150000</v>
       </c>
-      <c r="K6" s="395" t="s">
+      <c r="K6" s="397" t="s">
         <v>98</v>
       </c>
-      <c r="L6" s="396"/>
+      <c r="L6" s="398"/>
       <c r="M6" s="141">
         <v>1</v>
       </c>
@@ -5570,7 +5591,7 @@
     <mergeCell ref="M4:O4"/>
     <mergeCell ref="P4:P5"/>
   </mergeCells>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5606,31 +5627,31 @@
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B3" s="397" t="s">
+      <c r="B3" s="399" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="391"/>
-      <c r="D3" s="399" t="s">
+      <c r="C3" s="393"/>
+      <c r="D3" s="401" t="s">
         <v>85</v>
       </c>
-      <c r="E3" s="399"/>
-      <c r="F3" s="399"/>
-      <c r="G3" s="391" t="s">
+      <c r="E3" s="401"/>
+      <c r="F3" s="401"/>
+      <c r="G3" s="393" t="s">
         <v>89</v>
       </c>
-      <c r="H3" s="391" t="s">
+      <c r="H3" s="393" t="s">
         <v>90</v>
       </c>
-      <c r="I3" s="409" t="s">
+      <c r="I3" s="414" t="s">
         <v>93</v>
       </c>
-      <c r="J3" s="407" t="s">
+      <c r="J3" s="412" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="4" spans="2:15" s="137" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="413"/>
-      <c r="C4" s="411"/>
+      <c r="B4" s="408"/>
+      <c r="C4" s="409"/>
       <c r="D4" s="386" t="s">
         <v>86</v>
       </c>
@@ -5640,13 +5661,13 @@
       <c r="F4" s="386" t="s">
         <v>88</v>
       </c>
-      <c r="G4" s="411"/>
-      <c r="H4" s="411"/>
-      <c r="I4" s="410"/>
-      <c r="J4" s="408"/>
+      <c r="G4" s="409"/>
+      <c r="H4" s="409"/>
+      <c r="I4" s="415"/>
+      <c r="J4" s="413"/>
     </row>
     <row r="5" spans="2:15" s="342" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="404" t="s">
+      <c r="B5" s="402" t="s">
         <v>358</v>
       </c>
       <c r="C5" s="365" t="s">
@@ -5678,7 +5699,7 @@
       </c>
     </row>
     <row r="6" spans="2:15" s="137" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="406"/>
+      <c r="B6" s="404"/>
       <c r="C6" s="357" t="s">
         <v>360</v>
       </c>
@@ -5706,7 +5727,7 @@
       <c r="J6" s="361"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B7" s="404" t="s">
+      <c r="B7" s="402" t="s">
         <v>94</v>
       </c>
       <c r="C7" s="139" t="s">
@@ -5748,7 +5769,7 @@
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B8" s="405"/>
+      <c r="B8" s="407"/>
       <c r="C8" s="346" t="s">
         <v>91</v>
       </c>
@@ -5776,7 +5797,7 @@
       <c r="J8" s="363"/>
     </row>
     <row r="9" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="406"/>
+      <c r="B9" s="404"/>
       <c r="C9" s="350" t="s">
         <v>92</v>
       </c>
@@ -5804,7 +5825,7 @@
       <c r="J9" s="364"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B10" s="404" t="s">
+      <c r="B10" s="402" t="s">
         <v>96</v>
       </c>
       <c r="C10" s="139" t="s">
@@ -5834,7 +5855,7 @@
       <c r="J10" s="362"/>
     </row>
     <row r="11" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="405"/>
+      <c r="B11" s="407"/>
       <c r="C11" s="346" t="s">
         <v>362</v>
       </c>
@@ -5862,7 +5883,7 @@
       <c r="J11" s="363"/>
     </row>
     <row r="12" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="405"/>
+      <c r="B12" s="407"/>
       <c r="C12" s="346" t="s">
         <v>363</v>
       </c>
@@ -5890,7 +5911,7 @@
       <c r="J12" s="363"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B13" s="405"/>
+      <c r="B13" s="407"/>
       <c r="C13" s="346" t="s">
         <v>91</v>
       </c>
@@ -5918,7 +5939,7 @@
       <c r="J13" s="363"/>
     </row>
     <row r="14" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="406"/>
+      <c r="B14" s="404"/>
       <c r="C14" s="350" t="s">
         <v>92</v>
       </c>
@@ -5963,28 +5984,28 @@
     </row>
     <row r="23" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B24" s="404" t="s">
+      <c r="B24" s="402" t="s">
         <v>95</v>
       </c>
-      <c r="C24" s="400"/>
-      <c r="D24" s="412" t="s">
+      <c r="C24" s="403"/>
+      <c r="D24" s="406" t="s">
         <v>85</v>
       </c>
-      <c r="E24" s="412"/>
-      <c r="F24" s="412"/>
-      <c r="G24" s="400" t="s">
+      <c r="E24" s="406"/>
+      <c r="F24" s="406"/>
+      <c r="G24" s="403" t="s">
         <v>89</v>
       </c>
-      <c r="H24" s="400" t="s">
+      <c r="H24" s="403" t="s">
         <v>90</v>
       </c>
-      <c r="I24" s="402" t="s">
+      <c r="I24" s="410" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="25" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="406"/>
-      <c r="C25" s="401"/>
+      <c r="B25" s="404"/>
+      <c r="C25" s="405"/>
       <c r="D25" s="138" t="s">
         <v>86</v>
       </c>
@@ -5994,15 +6015,15 @@
       <c r="F25" s="138" t="s">
         <v>88</v>
       </c>
-      <c r="G25" s="401"/>
-      <c r="H25" s="401"/>
-      <c r="I25" s="403"/>
+      <c r="G25" s="405"/>
+      <c r="H25" s="405"/>
+      <c r="I25" s="411"/>
     </row>
     <row r="26" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="395" t="s">
+      <c r="B26" s="397" t="s">
         <v>99</v>
       </c>
-      <c r="C26" s="396"/>
+      <c r="C26" s="398"/>
       <c r="D26" s="141">
         <v>3</v>
       </c>
@@ -6043,11 +6064,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B24:C25"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B3:C4"/>
     <mergeCell ref="G24:G25"/>
     <mergeCell ref="H24:H25"/>
     <mergeCell ref="I24:I25"/>
@@ -6058,8 +6074,13 @@
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="G3:G4"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B24:C25"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B3:C4"/>
   </mergeCells>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -6712,7 +6733,7 @@
       <c r="K32" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
@@ -8029,7 +8050,7 @@
     </row>
   </sheetData>
   <autoFilter ref="B4:F4"/>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -9361,7 +9382,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
@@ -9924,7 +9945,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
@@ -10027,22 +10048,22 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="395" t="s">
+      <c r="C9" s="397" t="s">
         <v>347</v>
       </c>
-      <c r="D9" s="396"/>
-      <c r="E9" s="414">
+      <c r="D9" s="398"/>
+      <c r="E9" s="416">
         <f>SUM(F7:F8)</f>
         <v>620000</v>
       </c>
-      <c r="F9" s="415"/>
+      <c r="F9" s="417"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="C9:D9"/>
   </mergeCells>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -10051,7 +10072,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J45" sqref="J45"/>
     </sheetView>
@@ -11700,8 +11721,8 @@
       <c r="Q44" s="1"/>
     </row>
     <row r="45" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B45" s="420" t="s">
-        <v>391</v>
+      <c r="B45" s="392" t="s">
+        <v>390</v>
       </c>
       <c r="C45" s="234"/>
       <c r="D45" s="311" t="s">
@@ -11729,8 +11750,8 @@
       </c>
       <c r="M45" s="294"/>
       <c r="N45" s="34"/>
-      <c r="O45" s="419" t="s">
-        <v>390</v>
+      <c r="O45" s="391" t="s">
+        <v>389</v>
       </c>
       <c r="P45" s="39" t="s">
         <v>9</v>
@@ -12101,7 +12122,7 @@
   <sortState ref="B48:W53">
     <sortCondition ref="B48:B53"/>
   </sortState>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
[DOC] 구매 목록 update
</commit_message>
<xml_diff>
--- a/Femto Project 비용 List.xlsx
+++ b/Femto Project 비용 List.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3735" yWindow="1890" windowWidth="28800" windowHeight="12060" activeTab="1"/>
+    <workbookView xWindow="3735" yWindow="1890" windowWidth="28800" windowHeight="12060" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="전체 비용 List" sheetId="9" r:id="rId1"/>
@@ -18,16 +18,17 @@
     <sheet name="부품 list" sheetId="14" r:id="rId9"/>
     <sheet name="작업비" sheetId="11" r:id="rId10"/>
     <sheet name="0508" sheetId="16" r:id="rId11"/>
+    <sheet name="Sheet1" sheetId="17" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4">'0314'!$B$4:$F$4</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1219" uniqueCount="469">
   <si>
     <t>Vendor</t>
   </si>
@@ -1685,6 +1686,98 @@
   <si>
     <t>P007112027</t>
     <phoneticPr fontId="35" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMBT2222</t>
+  </si>
+  <si>
+    <t>NXP</t>
+  </si>
+  <si>
+    <t>Bipolar Transistors - BJT NPN SW 600MA 40V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P007250454 </t>
+    <phoneticPr fontId="35" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pipette Main</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>10K</t>
+  </si>
+  <si>
+    <t>WALSIN</t>
+  </si>
+  <si>
+    <t>RES SMD 10K OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P001909482 </t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.1uF</t>
+  </si>
+  <si>
+    <t>MURATA</t>
+  </si>
+  <si>
+    <t>CC1005-100nF50V(±10%/X7R)-(100개단위)</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>P008152676</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>CC1005-4.7uF10V(±20%/X5R)-(100개단위)</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.7uF</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>P008152648</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>P005627974</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>LF GEN MCU</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>51021-02</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>클림프 하우징/Board To Wire 1.25mm/Female/상대물:53047/핀수 2P</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>P005634320</t>
+    <phoneticPr fontId="35" type="noConversion"/>
+  </si>
+  <si>
+    <t>50058 양단 케이블 L=100mm, Red</t>
+    <phoneticPr fontId="35" type="noConversion"/>
+  </si>
+  <si>
+    <t>포밍테이블</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>1200x900 연체리 + 배송비 (7000원)</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>11번가</t>
+    <phoneticPr fontId="12" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3063,7 +3156,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="451">
+  <cellXfs count="465">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
@@ -4072,27 +4165,36 @@
     <xf numFmtId="0" fontId="30" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="33" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4105,15 +4207,6 @@
     <xf numFmtId="0" fontId="30" fillId="33" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="33" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="33" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="30" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4129,6 +4222,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="41" fontId="30" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="36" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="14" xfId="69" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="80" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="96">
     <cellStyle name="20% - 강조색1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5665,6 +5794,17 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="M37:O37"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="O42:P42"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="C22:E22"/>
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="E28:F28"/>
     <mergeCell ref="H9:J9"/>
@@ -5673,17 +5813,6 @@
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C15:D15"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="M23:O23"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="M37:O37"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="O42:P42"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5696,7 +5825,7 @@
   <dimension ref="A2:N24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="B14" sqref="B14:L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6291,11 +6420,373 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:P21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="56" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="210" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="81" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="81" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="81" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="211" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="408" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="81" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="81" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" s="82" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B4" s="185" t="s">
+        <v>444</v>
+      </c>
+      <c r="C4" s="186" t="s">
+        <v>445</v>
+      </c>
+      <c r="D4" s="186" t="s">
+        <v>446</v>
+      </c>
+      <c r="E4" s="355"/>
+      <c r="F4" s="187">
+        <v>5</v>
+      </c>
+      <c r="G4" s="454">
+        <v>50</v>
+      </c>
+      <c r="H4" s="455">
+        <v>1</v>
+      </c>
+      <c r="I4" s="456">
+        <v>100</v>
+      </c>
+      <c r="J4" s="457">
+        <v>5000</v>
+      </c>
+      <c r="K4" s="457"/>
+      <c r="L4" s="405" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B5" s="134" t="s">
+        <v>449</v>
+      </c>
+      <c r="C5" s="180" t="s">
+        <v>450</v>
+      </c>
+      <c r="D5" s="180" t="s">
+        <v>451</v>
+      </c>
+      <c r="E5" s="348"/>
+      <c r="F5" s="298">
+        <v>14</v>
+      </c>
+      <c r="G5" s="349">
+        <v>10</v>
+      </c>
+      <c r="H5" s="348"/>
+      <c r="I5" s="348">
+        <v>200</v>
+      </c>
+      <c r="J5" s="349">
+        <f>G5*I5</f>
+        <v>2000</v>
+      </c>
+      <c r="K5" s="348"/>
+      <c r="L5" s="458" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B6" s="134" t="s">
+        <v>453</v>
+      </c>
+      <c r="C6" s="180" t="s">
+        <v>454</v>
+      </c>
+      <c r="D6" s="180" t="s">
+        <v>455</v>
+      </c>
+      <c r="E6" s="348"/>
+      <c r="F6" s="60">
+        <v>10</v>
+      </c>
+      <c r="G6" s="349">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H6" s="348"/>
+      <c r="I6" s="348">
+        <v>300</v>
+      </c>
+      <c r="J6" s="349">
+        <f>G6*I6</f>
+        <v>1530</v>
+      </c>
+      <c r="K6" s="348"/>
+      <c r="L6" s="89" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B7" s="459" t="s">
+        <v>458</v>
+      </c>
+      <c r="C7" s="180" t="s">
+        <v>454</v>
+      </c>
+      <c r="D7" s="58" t="s">
+        <v>457</v>
+      </c>
+      <c r="E7" s="348"/>
+      <c r="F7" s="348"/>
+      <c r="G7" s="349">
+        <v>5</v>
+      </c>
+      <c r="H7" s="348"/>
+      <c r="I7" s="348">
+        <v>200</v>
+      </c>
+      <c r="J7" s="349">
+        <f>G7*I7</f>
+        <v>1000</v>
+      </c>
+      <c r="K7" s="348"/>
+      <c r="L7" s="89" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="76" t="s">
+        <v>194</v>
+      </c>
+      <c r="C8" s="190" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="190" t="s">
+        <v>465</v>
+      </c>
+      <c r="E8" s="327"/>
+      <c r="F8" s="460"/>
+      <c r="G8" s="460">
+        <v>130</v>
+      </c>
+      <c r="H8" s="460">
+        <v>300</v>
+      </c>
+      <c r="I8" s="460">
+        <v>300</v>
+      </c>
+      <c r="J8" s="353">
+        <f>G8*I8</f>
+        <v>39000</v>
+      </c>
+      <c r="K8" s="36"/>
+      <c r="L8" s="418" t="s">
+        <v>195</v>
+      </c>
+      <c r="P8" s="39"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="G9" s="5"/>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="2:16" s="452" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="451" t="s">
+        <v>461</v>
+      </c>
+      <c r="J10" s="453"/>
+    </row>
+    <row r="11" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="210" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="81" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="81" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="81" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="211" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="408" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="81" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" s="81" t="s">
+        <v>7</v>
+      </c>
+      <c r="L11" s="82" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="461" t="s">
+        <v>462</v>
+      </c>
+      <c r="C12" s="462" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="104" t="s">
+        <v>463</v>
+      </c>
+      <c r="E12" s="104"/>
+      <c r="F12" s="104"/>
+      <c r="G12" s="142">
+        <v>250</v>
+      </c>
+      <c r="H12" s="104">
+        <v>10</v>
+      </c>
+      <c r="I12" s="104">
+        <v>10</v>
+      </c>
+      <c r="J12" s="142">
+        <f>G12*I12</f>
+        <v>2500</v>
+      </c>
+      <c r="K12" s="104"/>
+      <c r="L12" s="463" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="J15" s="11">
+        <f>SUM(J4:J14)</f>
+        <v>51030</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="J16" s="50">
+        <f>J15*0.1+J15</f>
+        <v>56133</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="210" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="81" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="81" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="81" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="211" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="408" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" s="81" t="s">
+        <v>5</v>
+      </c>
+      <c r="I20" s="81" t="s">
+        <v>20</v>
+      </c>
+      <c r="J20" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="K20" s="81" t="s">
+        <v>7</v>
+      </c>
+      <c r="L20" s="82" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="461" t="s">
+        <v>466</v>
+      </c>
+      <c r="C21" s="104"/>
+      <c r="D21" s="104" t="s">
+        <v>467</v>
+      </c>
+      <c r="E21" s="104"/>
+      <c r="F21" s="104"/>
+      <c r="G21" s="142">
+        <v>57600</v>
+      </c>
+      <c r="H21" s="104"/>
+      <c r="I21" s="104">
+        <v>1</v>
+      </c>
+      <c r="J21" s="142">
+        <f>G21*I21</f>
+        <v>57600</v>
+      </c>
+      <c r="K21" s="104"/>
+      <c r="L21" s="464" t="s">
+        <v>468</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="12" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
@@ -6870,16 +7361,16 @@
       <c r="H3" s="423" t="s">
         <v>90</v>
       </c>
-      <c r="I3" s="441" t="s">
+      <c r="I3" s="444" t="s">
         <v>93</v>
       </c>
-      <c r="J3" s="439" t="s">
+      <c r="J3" s="442" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="4" spans="2:15" s="137" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="445"/>
-      <c r="C4" s="443"/>
+      <c r="B4" s="438"/>
+      <c r="C4" s="439"/>
       <c r="D4" s="386" t="s">
         <v>86</v>
       </c>
@@ -6889,13 +7380,13 @@
       <c r="F4" s="386" t="s">
         <v>88</v>
       </c>
-      <c r="G4" s="443"/>
-      <c r="H4" s="443"/>
-      <c r="I4" s="442"/>
-      <c r="J4" s="440"/>
+      <c r="G4" s="439"/>
+      <c r="H4" s="439"/>
+      <c r="I4" s="445"/>
+      <c r="J4" s="443"/>
     </row>
     <row r="5" spans="2:15" s="342" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="436" t="s">
+      <c r="B5" s="432" t="s">
         <v>358</v>
       </c>
       <c r="C5" s="365" t="s">
@@ -6927,7 +7418,7 @@
       </c>
     </row>
     <row r="6" spans="2:15" s="137" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="438"/>
+      <c r="B6" s="434"/>
       <c r="C6" s="357" t="s">
         <v>360</v>
       </c>
@@ -6955,7 +7446,7 @@
       <c r="J6" s="361"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B7" s="436" t="s">
+      <c r="B7" s="432" t="s">
         <v>94</v>
       </c>
       <c r="C7" s="139" t="s">
@@ -7025,7 +7516,7 @@
       <c r="J8" s="363"/>
     </row>
     <row r="9" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="438"/>
+      <c r="B9" s="434"/>
       <c r="C9" s="350" t="s">
         <v>92</v>
       </c>
@@ -7053,7 +7544,7 @@
       <c r="J9" s="364"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B10" s="436" t="s">
+      <c r="B10" s="432" t="s">
         <v>96</v>
       </c>
       <c r="C10" s="139" t="s">
@@ -7167,7 +7658,7 @@
       <c r="J13" s="363"/>
     </row>
     <row r="14" spans="2:15" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="438"/>
+      <c r="B14" s="434"/>
       <c r="C14" s="350" t="s">
         <v>92</v>
       </c>
@@ -7212,28 +7703,28 @@
     </row>
     <row r="23" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B24" s="436" t="s">
+      <c r="B24" s="432" t="s">
         <v>95</v>
       </c>
-      <c r="C24" s="432"/>
-      <c r="D24" s="444" t="s">
+      <c r="C24" s="433"/>
+      <c r="D24" s="436" t="s">
         <v>85</v>
       </c>
-      <c r="E24" s="444"/>
-      <c r="F24" s="444"/>
-      <c r="G24" s="432" t="s">
+      <c r="E24" s="436"/>
+      <c r="F24" s="436"/>
+      <c r="G24" s="433" t="s">
         <v>89</v>
       </c>
-      <c r="H24" s="432" t="s">
+      <c r="H24" s="433" t="s">
         <v>90</v>
       </c>
-      <c r="I24" s="434" t="s">
+      <c r="I24" s="440" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="25" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="438"/>
-      <c r="C25" s="433"/>
+      <c r="B25" s="434"/>
+      <c r="C25" s="435"/>
       <c r="D25" s="138" t="s">
         <v>86</v>
       </c>
@@ -7243,9 +7734,9 @@
       <c r="F25" s="138" t="s">
         <v>88</v>
       </c>
-      <c r="G25" s="433"/>
-      <c r="H25" s="433"/>
-      <c r="I25" s="435"/>
+      <c r="G25" s="435"/>
+      <c r="H25" s="435"/>
+      <c r="I25" s="441"/>
     </row>
     <row r="26" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="427" t="s">
@@ -7292,11 +7783,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B24:C25"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B3:C4"/>
     <mergeCell ref="G24:G25"/>
     <mergeCell ref="H24:H25"/>
     <mergeCell ref="I24:I25"/>
@@ -7307,6 +7793,11 @@
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="G3:G4"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B24:C25"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B3:C4"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7971,8 +8462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N42" sqref="N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -9246,7 +9737,7 @@
         <v>39000</v>
       </c>
       <c r="N36" s="193" t="s">
-        <v>195</v>
+        <v>464</v>
       </c>
     </row>
     <row r="37" spans="1:14" s="177" customFormat="1" x14ac:dyDescent="0.3">
@@ -11301,8 +11792,8 @@
   <dimension ref="B2:R55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H39" sqref="H39"/>
+      <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>